<commit_message>
Code for Ui Automation
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\eclipse-workspace\WellFrontendTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Promantus\git\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0564072-0881-4DA2-B77F-993CB5080378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F5809C-8F70-4DAD-B54B-B7DDA945BF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="10680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Portfolio" sheetId="2" r:id="rId2"/>
+    <sheet name="Faculty" sheetId="7" r:id="rId3"/>
+    <sheet name="V2Project" sheetId="3" r:id="rId4"/>
+    <sheet name="exam" sheetId="6" r:id="rId5"/>
+    <sheet name="Hsr" sheetId="4" r:id="rId6"/>
+    <sheet name="Wpr" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>UserName</t>
   </si>
@@ -58,148 +63,106 @@
     <t>OrgIndustry</t>
   </si>
   <si>
-    <t>Packing &amp; Shipping</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1715570</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2228462</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1967170</t>
-  </si>
-  <si>
-    <t>Medical Support</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2620072</t>
-  </si>
-  <si>
-    <t>Air Travel</t>
-  </si>
-  <si>
-    <t>Automation portfolio 5634494</t>
-  </si>
-  <si>
-    <t>Multifamily Housing (market rate)</t>
-  </si>
-  <si>
-    <t>Automation portfolio 7909732</t>
-  </si>
-  <si>
-    <t>Community</t>
-  </si>
-  <si>
-    <t>Automation portfolio 634910</t>
-  </si>
-  <si>
-    <t>Automation portfolio 3448560</t>
-  </si>
-  <si>
-    <t>Affordable Housing</t>
-  </si>
-  <si>
-    <t>Automation portfolio 5662475</t>
-  </si>
-  <si>
-    <t>Investment Services</t>
-  </si>
-  <si>
-    <t>Automation portfolio 941518</t>
-  </si>
-  <si>
-    <t>Travel Support</t>
-  </si>
-  <si>
-    <t>Automation portfolio 6983211</t>
-  </si>
-  <si>
-    <t>Sports</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2762201</t>
-  </si>
-  <si>
-    <t>Sustainability</t>
-  </si>
-  <si>
-    <t>Automation portfolio 269831</t>
-  </si>
-  <si>
-    <t>Student Housing</t>
-  </si>
-  <si>
-    <t>Automation portfolio 543252</t>
-  </si>
-  <si>
-    <t>Automation portfolio 4912993</t>
-  </si>
-  <si>
-    <t>Energy Production</t>
-  </si>
-  <si>
-    <t>Automation portfolio 571586</t>
-  </si>
-  <si>
-    <t>Hospitals</t>
-  </si>
-  <si>
-    <t>Automation portfolio 7466534</t>
-  </si>
-  <si>
-    <t>Automation portfolio 4076636</t>
-  </si>
-  <si>
-    <t>Telecommunications</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2873100</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2353978</t>
-  </si>
-  <si>
-    <t>Building Services</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1955855</t>
-  </si>
-  <si>
-    <t>Automation portfolio 6852301</t>
-  </si>
-  <si>
-    <t>Materials &amp; Chemicals</t>
-  </si>
-  <si>
-    <t>Automation portfolio 410931</t>
-  </si>
-  <si>
-    <t>Accounting</t>
-  </si>
-  <si>
-    <t>Automation portfolio 6513800</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1205735</t>
+    <t>projectId</t>
+  </si>
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>hsrId</t>
+  </si>
+  <si>
+    <t>hsrName</t>
   </si>
   <si>
     <t>Restaurant</t>
   </si>
   <si>
-    <t>Automation portfolio 2131913</t>
-  </si>
-  <si>
-    <t>Education Support</t>
-  </si>
-  <si>
-    <t>Automation portfolio 707334</t>
+    <t>Automation portfolio 3036770</t>
+  </si>
+  <si>
+    <t>REIT</t>
+  </si>
+  <si>
+    <t>Automation Project4253865</t>
+  </si>
+  <si>
+    <t>2202263557</t>
+  </si>
+  <si>
+    <t>Automation Project5647617</t>
+  </si>
+  <si>
+    <t>2202263660</t>
+  </si>
+  <si>
+    <t>Automation Project1358995</t>
+  </si>
+  <si>
+    <t>2202263699</t>
+  </si>
+  <si>
+    <t>Automation Project5652127</t>
+  </si>
+  <si>
+    <t>2202263700</t>
+  </si>
+  <si>
+    <t>Automation Project3317483</t>
+  </si>
+  <si>
+    <t>2202263701</t>
+  </si>
+  <si>
+    <t>Automation Project7786158</t>
+  </si>
+  <si>
+    <t>2202263702</t>
+  </si>
+  <si>
+    <t>Automation Project864000</t>
+  </si>
+  <si>
+    <t>2202263703</t>
+  </si>
+  <si>
+    <t>Automation Project1664091</t>
+  </si>
+  <si>
+    <t>2202263704</t>
+  </si>
+  <si>
+    <t>Automation Project4468000</t>
+  </si>
+  <si>
+    <t>2202263709</t>
+  </si>
+  <si>
+    <t>Automation Project4318943</t>
+  </si>
+  <si>
+    <t>2202263744</t>
+  </si>
+  <si>
+    <t>Automation Project1233869</t>
+  </si>
+  <si>
+    <t>2202263745</t>
   </si>
 </sst>
 </file>
@@ -245,9 +208,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -535,13 +499,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -552,12 +516,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -568,7 +532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -585,18 +549,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA429754-6532-434F-8D5F-1B15F28EE35F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.60546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -604,12 +568,211 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCA1BAA-A15F-4FC5-B79A-8DB6B7F32D60}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DDA08-C4FB-4E43-ADE7-EDDAA41E68CF}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.38671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35500AA9-B12B-4C68-9D48-7FBAC0E91A3C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F8409-99F8-4FFC-AA3A-80D15FF5718E}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6328ECB3-CDE0-459F-815E-F1AAB0123146}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code for V2project,Exam and Wpr
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D464AE-F9BF-4BF9-9D53-C4ABA940380E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E4520E-42E6-4E80-A832-405925E60806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
   <si>
     <t>UserName</t>
   </si>
@@ -64,9 +64,6 @@
     <t>OrgIndustry</t>
   </si>
   <si>
-    <t>projectId</t>
-  </si>
-  <si>
     <t>projectName</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Karnataka</t>
   </si>
   <si>
-    <t>area</t>
-  </si>
-  <si>
     <t>hsrId</t>
   </si>
   <si>
@@ -130,51 +124,6 @@
     <t>IWBI</t>
   </si>
   <si>
-    <t>Automation WPR Project837598</t>
-  </si>
-  <si>
-    <t>WPR006029</t>
-  </si>
-  <si>
-    <t>w632afdbd74a7d</t>
-  </si>
-  <si>
-    <t>Senior Living, Assisted Living, Skilled Nursing Facility</t>
-  </si>
-  <si>
-    <t>HSRP006031</t>
-  </si>
-  <si>
-    <t>Automation V2 Project3841643</t>
-  </si>
-  <si>
-    <t>Automation portfolio 314289</t>
-  </si>
-  <si>
-    <t>Affordable Housing</t>
-  </si>
-  <si>
-    <t>2202265791</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2262392</t>
-  </si>
-  <si>
-    <t>Clinical Services</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1599053</t>
-  </si>
-  <si>
-    <t>Medical Support</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1709920</t>
-  </si>
-  <si>
-    <t>Insurance</t>
-  </si>
-  <si>
     <t>Automation portfolio 2745982</t>
   </si>
   <si>
@@ -187,16 +136,226 @@
     <t>HSRP006109</t>
   </si>
   <si>
-    <t>Automation V2 Project4546628</t>
-  </si>
-  <si>
-    <t>2202266249</t>
-  </si>
-  <si>
-    <t>Automation V2 Project1487962</t>
-  </si>
-  <si>
-    <t>2202266256</t>
+    <t>ProjectId</t>
+  </si>
+  <si>
+    <t>ProjectName</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Org</t>
+  </si>
+  <si>
+    <t>OwnerName</t>
+  </si>
+  <si>
+    <t>OwnerEmail</t>
+  </si>
+  <si>
+    <t>CardHolderName</t>
+  </si>
+  <si>
+    <t>CardHolderNumber</t>
+  </si>
+  <si>
+    <t>CardHolderExpDate</t>
+  </si>
+  <si>
+    <t>CardHolderCVC</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>PhoneNum</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>WPRSelectMember</t>
+  </si>
+  <si>
+    <t>WPRlocations</t>
+  </si>
+  <si>
+    <t>WPRlocationsize</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>https://test-nuxt.wellcertified.com/projects/v2/2202266385/register</t>
+  </si>
+  <si>
+    <t>4111 1111 1111 1111</t>
+  </si>
+  <si>
+    <t>09 / 25</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>Automation V2 Project6977806</t>
+  </si>
+  <si>
+    <t>1442</t>
+  </si>
+  <si>
+    <t>2202266393</t>
+  </si>
+  <si>
+    <t>100 RESILIENT CITIES</t>
+  </si>
+  <si>
+    <t>Lawerence</t>
+  </si>
+  <si>
+    <t>krystina.daniel@hotmail.com</t>
+  </si>
+  <si>
+    <t>5152552350</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>530 Fahey Orchard</t>
+  </si>
+  <si>
+    <t>North Leroymouth</t>
+  </si>
+  <si>
+    <t>34233</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>Automation WPR Project815339</t>
+  </si>
+  <si>
+    <t>101 Projects</t>
+  </si>
+  <si>
+    <t>Consultancies</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>16146 Merle Harbors</t>
+  </si>
+  <si>
+    <t>New Olinfurt</t>
+  </si>
+  <si>
+    <t>32547</t>
+  </si>
+  <si>
+    <t>WPR006168</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>APJobtitle</t>
+  </si>
+  <si>
+    <t>APIndustry</t>
+  </si>
+  <si>
+    <t>APSelectWELLAP</t>
+  </si>
+  <si>
+    <t>APLanguage</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>8678 Heathcote Canyon</t>
+  </si>
+  <si>
+    <t>Port Collette</t>
+  </si>
+  <si>
+    <t>06283-3941</t>
+  </si>
+  <si>
+    <t>2578481302</t>
+  </si>
+  <si>
+    <t>Neil</t>
+  </si>
+  <si>
+    <t>w633303faa09a8</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>9641 Bechtelar Extension</t>
+  </si>
+  <si>
+    <t>South Regan</t>
+  </si>
+  <si>
+    <t>14021-0356</t>
+  </si>
+  <si>
+    <t>1247711361</t>
+  </si>
+  <si>
+    <t>Edmundo</t>
+  </si>
+  <si>
+    <t>010110 Architecture + Urbanism</t>
+  </si>
+  <si>
+    <t>Aerospace &amp; Aviation</t>
+  </si>
+  <si>
+    <t>Delos</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Colby</t>
+  </si>
+  <si>
+    <t>w633305715c722</t>
   </si>
 </sst>
 </file>
@@ -561,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -602,8 +761,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.6796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="28.5703125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -617,10 +776,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -640,18 +799,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -661,51 +820,151 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DDA08-C4FB-4E43-ADE7-EDDAA41E68CF}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.37109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.8359375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -715,37 +974,102 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35500AA9-B12B-4C68-9D48-7FBAC0E91A3C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.2578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.51953125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.33984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.04296875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.828125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.95703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -764,39 +1088,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="47.31640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -806,44 +1130,102 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6328ECB3-CDE0-459F-815E-F1AAB0123146}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -869,51 +1251,51 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
       </c>
       <c r="E2">
         <v>9099099990</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code modification for Testdata
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E4520E-42E6-4E80-A832-405925E60806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5407C2-AF4C-4500-911F-7EEB58441D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
   <si>
     <t>UserName</t>
   </si>
@@ -301,61 +301,73 @@
     <t>APLanguage</t>
   </si>
   <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>9641 Bechtelar Extension</t>
+  </si>
+  <si>
+    <t>South Regan</t>
+  </si>
+  <si>
+    <t>14021-0356</t>
+  </si>
+  <si>
+    <t>1247711361</t>
+  </si>
+  <si>
+    <t>Edmundo</t>
+  </si>
+  <si>
+    <t>010110 Architecture + Urbanism</t>
+  </si>
+  <si>
+    <t>Aerospace &amp; Aviation</t>
+  </si>
+  <si>
+    <t>Delos</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Colby</t>
+  </si>
+  <si>
+    <t>w633305715c722</t>
+  </si>
+  <si>
+    <t>WFEmp</t>
+  </si>
+  <si>
+    <t>WFPostion</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>321 Rowe Tunnel</t>
+  </si>
+  <si>
+    <t>Wisokyview</t>
+  </si>
+  <si>
+    <t>99998-0972</t>
+  </si>
+  <si>
+    <t>FullTime</t>
+  </si>
+  <si>
     <t>Michigan</t>
   </si>
   <si>
-    <t>8678 Heathcote Canyon</t>
-  </si>
-  <si>
-    <t>Port Collette</t>
-  </si>
-  <si>
-    <t>06283-3941</t>
-  </si>
-  <si>
-    <t>2578481302</t>
-  </si>
-  <si>
-    <t>Neil</t>
-  </si>
-  <si>
-    <t>w633303faa09a8</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>9641 Bechtelar Extension</t>
-  </si>
-  <si>
-    <t>South Regan</t>
-  </si>
-  <si>
-    <t>14021-0356</t>
-  </si>
-  <si>
-    <t>1247711361</t>
-  </si>
-  <si>
-    <t>Edmundo</t>
-  </si>
-  <si>
-    <t>010110 Architecture + Urbanism</t>
-  </si>
-  <si>
-    <t>Aerospace &amp; Aviation</t>
-  </si>
-  <si>
-    <t>Delos</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Colby</t>
-  </si>
-  <si>
-    <t>w633305715c722</t>
+    <t>06507 Marylynn Ford</t>
+  </si>
+  <si>
+    <t>DuBuqueborough</t>
+  </si>
+  <si>
+    <t>26329</t>
   </si>
 </sst>
 </file>
@@ -789,28 +801,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCA1BAA-A15F-4FC5-B79A-8DB6B7F32D60}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5390625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.68359375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.2421875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.64453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.71875" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -823,7 +881,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -843,10 +901,10 @@
     <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.37109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.8359375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -955,7 +1013,7 @@
         <v>64</v>
       </c>
       <c r="P2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="Q2" t="s">
         <v>57</v>
@@ -976,24 +1034,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35500AA9-B12B-4C68-9D48-7FBAC0E91A3C}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.2578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.51953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.33984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.04296875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.828125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.95703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="4.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1036,40 +1094,40 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>78</v>
       </c>
       <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" t="s">
         <v>96</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
         <v>97</v>
       </c>
-      <c r="F2" t="s">
+      <c r="L2" t="s">
         <v>98</v>
-      </c>
-      <c r="G2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L2" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code fix for Org
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025649C9-AAD5-47CC-82D6-92D9A9B89925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463951CE-26A8-4F9B-B595-17B46824DE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="129">
   <si>
     <t>UserName</t>
   </si>
@@ -385,17 +385,46 @@
     <t>OwnerPhone</t>
   </si>
   <si>
-    <t>Automation portfolio 1630196</t>
-  </si>
-  <si>
-    <t>Automation portfolio 3896680</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Joey</t>
+  </si>
+  <si>
+    <t>jayne.keebler@hotmail.com</t>
+  </si>
+  <si>
+    <t>7362255383</t>
+  </si>
+  <si>
+    <t>Automation portfolio 4377747</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>26556</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>88741 Lucas Locks</t>
+  </si>
+  <si>
+    <t>Durganberg</t>
+  </si>
+  <si>
+    <t>59989-8155</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -733,8 +762,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -788,17 +817,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA429754-6532-434F-8D5F-1B15F28EE35F}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -845,9 +883,48 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
         <v>118</v>
+      </c>
+      <c r="F2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -857,24 +934,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCA1BAA-A15F-4FC5-B79A-8DB6B7F32D60}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -899,8 +976,11 @@
       <c r="H1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -941,25 +1021,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1095,18 +1175,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1193,19 +1273,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F8409-99F8-4FFC-AA3A-80D15FF5718E}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1221,8 +1301,11 @@
       <c r="E1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1251,18 +1334,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1356,16 +1439,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>

<commit_message>
code fix for support
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91735\Documents\Project WellCertified\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025649C9-AAD5-47CC-82D6-92D9A9B89925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D404D431-D54C-4603-8573-10B4ED459056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
   <si>
     <t>UserName</t>
   </si>
@@ -187,9 +187,6 @@
     <t>1442</t>
   </si>
   <si>
-    <t>2202266393</t>
-  </si>
-  <si>
     <t>100 RESILIENT CITIES</t>
   </si>
   <si>
@@ -385,10 +382,52 @@
     <t>OwnerPhone</t>
   </si>
   <si>
-    <t>Automation portfolio 1630196</t>
-  </si>
-  <si>
-    <t>Automation portfolio 3896680</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Joey</t>
+  </si>
+  <si>
+    <t>jayne.keebler@hotmail.com</t>
+  </si>
+  <si>
+    <t>7362255383</t>
+  </si>
+  <si>
+    <t>Automation portfolio 4377747</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>26556</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>88741 Lucas Locks</t>
+  </si>
+  <si>
+    <t>Durganberg</t>
+  </si>
+  <si>
+    <t>59989-8155</t>
+  </si>
+  <si>
+    <t>FeatureName</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>2202266502</t>
+  </si>
+  <si>
+    <t>A01 Air Quality</t>
   </si>
 </sst>
 </file>
@@ -439,11 +478,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -731,10 +771,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -788,17 +828,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA429754-6532-434F-8D5F-1B15F28EE35F}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -809,16 +858,16 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>114</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
       </c>
       <c r="G1" t="s">
         <v>25</v>
@@ -842,12 +891,51 @@
         <v>30</v>
       </c>
       <c r="N1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" t="s">
         <v>118</v>
+      </c>
+      <c r="M2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -857,24 +945,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCA1BAA-A15F-4FC5-B79A-8DB6B7F32D60}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.26953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -891,36 +979,39 @@
         <v>37</v>
       </c>
       <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
         <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" t="s">
-        <v>92</v>
       </c>
       <c r="H2" t="s">
         <v>20</v>
@@ -933,36 +1024,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DDA08-C4FB-4E43-ADE7-EDDAA41E68CF}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.7265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="4.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.81640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.453125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7265625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="13.27734375" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1020,31 +1112,37 @@
       <c r="S1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" t="s">
-        <v>51</v>
+      <c r="T1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
       </c>
       <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
         <v>57</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>59</v>
-      </c>
-      <c r="H2" t="s">
-        <v>60</v>
       </c>
       <c r="I2" t="s">
         <v>45</v>
@@ -1053,22 +1151,22 @@
         <v>50</v>
       </c>
       <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
         <v>52</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>53</v>
       </c>
-      <c r="M2" t="s">
-        <v>54</v>
-      </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q2" t="s">
         <v>46</v>
@@ -1079,9 +1177,13 @@
       <c r="S2" t="s">
         <v>48</v>
       </c>
+      <c r="T2" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1093,19 +1195,19 @@
       <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.26953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="4.26953125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
@@ -1114,7 +1216,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
         <v>25</v>
@@ -1132,57 +1234,57 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I1" t="s">
         <v>28</v>
       </c>
       <c r="J1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" t="s">
         <v>75</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>76</v>
-      </c>
-      <c r="L1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>83</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>84</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>85</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>86</v>
-      </c>
-      <c r="L2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1193,19 +1295,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F8409-99F8-4FFC-AA3A-80D15FF5718E}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.453125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="47.26953125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1221,8 +1323,11 @@
       <c r="E1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1249,20 +1354,20 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.26953125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1305,40 +1410,40 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>69</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>70</v>
       </c>
-      <c r="I2" t="s">
-        <v>71</v>
-      </c>
       <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
         <v>61</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>62</v>
-      </c>
-      <c r="L2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1354,32 +1459,32 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.54296875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="4.453125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" t="s">
-        <v>98</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
@@ -1388,10 +1493,10 @@
         <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" t="s">
         <v>36</v>
@@ -1402,34 +1507,34 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
         <v>44</v>
       </c>
       <c r="F2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" t="s">
         <v>108</v>
-      </c>
-      <c r="G2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J2" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testdata changes for Hsr
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91735\Documents\Project WellCertified\WellFrontendTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D404D431-D54C-4603-8573-10B4ED459056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3A8022-0B13-4C46-B54D-CFA09F98363A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
   <si>
     <t>UserName</t>
   </si>
@@ -67,24 +67,9 @@
     <t>projectName</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
-  </si>
-  <si>
     <t>hsrId</t>
   </si>
   <si>
-    <t>hsrName</t>
-  </si>
-  <si>
     <t>testuserdevid@gmail.com</t>
   </si>
   <si>
@@ -97,9 +82,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>REIT</t>
-  </si>
-  <si>
     <t>HSRP006109</t>
   </si>
   <si>
@@ -428,13 +410,36 @@
   </si>
   <si>
     <t>A01 Air Quality</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>71857 Schmitt Lane</t>
+  </si>
+  <si>
+    <t>Baumbachfurt</t>
+  </si>
+  <si>
+    <t>81146</t>
+  </si>
+  <si>
+    <t>023854</t>
+  </si>
+  <si>
+    <t>HsrName</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 842536</t>
+  </si>
+  <si>
+    <t>Fitness &amp; Recreation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -478,12 +483,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -771,10 +775,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.81640625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -793,7 +797,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -832,22 +836,22 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.7265625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -858,84 +862,84 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" t="s">
         <v>121</v>
       </c>
-      <c r="B2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K2" t="s">
-        <v>127</v>
-      </c>
       <c r="L2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="M2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="N2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -951,70 +955,70 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1026,159 +1030,159 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DDA08-C4FB-4E43-ADE7-EDDAA41E68CF}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.7265625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="4.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.81640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="24.453125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.453125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7265625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.27734375" collapsed="false"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>30</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
       </c>
       <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>122</v>
+      </c>
+      <c r="U1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2" t="s">
         <v>40</v>
       </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" t="s">
-        <v>128</v>
-      </c>
-      <c r="U1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>46</v>
-      </c>
       <c r="R2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="S2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1195,96 +1199,96 @@
       <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.26953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.26953125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="K1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>78</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>80</v>
-      </c>
-      <c r="H2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L2" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1295,50 +1299,95 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F8409-99F8-4FFC-AA3A-80D15FF5718E}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.453125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="47.26953125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
+      <c r="B2" t="s">
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1354,96 +1403,96 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" t="s">
-        <v>70</v>
-      </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1459,82 +1508,82 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.7265625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.453125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s">
         <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J2" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code fix exam and hsr
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="180">
   <si>
     <t>UserName</t>
   </si>
@@ -434,12 +434,151 @@
   </si>
   <si>
     <t>Fitness &amp; Recreation</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 2950373</t>
+  </si>
+  <si>
+    <t>Retirement Communities</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>46273 Klein Valley</t>
+  </si>
+  <si>
+    <t>Joesphhaven</t>
+  </si>
+  <si>
+    <t>54976-8486</t>
+  </si>
+  <si>
+    <t>010998</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 1614551</t>
+  </si>
+  <si>
+    <t>100 Percent Group Limited</t>
+  </si>
+  <si>
+    <t>Air Travel</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>68192 Boehm Walks</t>
+  </si>
+  <si>
+    <t>Arielhaven</t>
+  </si>
+  <si>
+    <t>31332-2867</t>
+  </si>
+  <si>
+    <t>015029</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 7528778</t>
+  </si>
+  <si>
+    <t>101 Moorgate</t>
+  </si>
+  <si>
+    <t>Hospitals</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>7937 Carson Ports</t>
+  </si>
+  <si>
+    <t>Donberg</t>
+  </si>
+  <si>
+    <t>48982</t>
+  </si>
+  <si>
+    <t>01517</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 1227587</t>
+  </si>
+  <si>
+    <t>Post Secondary Education</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>812 Monserrate Underpass</t>
+  </si>
+  <si>
+    <t>Port Jodishire</t>
+  </si>
+  <si>
+    <t>18123</t>
+  </si>
+  <si>
+    <t>017176</t>
+  </si>
+  <si>
+    <t>Gregorio</t>
+  </si>
+  <si>
+    <t>HSRP006238</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 7162135</t>
+  </si>
+  <si>
+    <t>1-800 Flowers.com Inc.</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>074 Krystyna Shoal</t>
+  </si>
+  <si>
+    <t>Chantayburgh</t>
+  </si>
+  <si>
+    <t>00030-5564</t>
+  </si>
+  <si>
+    <t>015332</t>
+  </si>
+  <si>
+    <t>Norris</t>
+  </si>
+  <si>
+    <t>6935 Lizette Ridges</t>
+  </si>
+  <si>
+    <t>West Marinda</t>
+  </si>
+  <si>
+    <t>95210</t>
+  </si>
+  <si>
+    <t>1830104860</t>
+  </si>
+  <si>
+    <t>Wilburn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -777,8 +916,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -838,20 +977,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -957,13 +1096,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1036,26 +1175,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.37109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.8359375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -1170,7 +1309,7 @@
         <v>46</v>
       </c>
       <c r="P2" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="Q2" t="s">
         <v>40</v>
@@ -1201,18 +1340,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.04296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.72265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.2890625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.04296875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.12890625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.3046875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1258,28 +1397,28 @@
         <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>179</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
         <v>78</v>
@@ -1307,17 +1446,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="30.95703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.6953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.95703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.46484375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.2421875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1357,37 +1496,37 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="G2" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="H2" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="J2" t="s">
         <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>130</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1405,18 +1544,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1510,16 +1649,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>

<commit_message>
Code fix for review
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\eclipse-workspace\WellFrontendTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6AA70B-5F5C-4667-B2A6-6121265335F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EADF7F6-B828-4063-978B-E1885BC52261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="3756" windowWidth="17280" windowHeight="10680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="137">
   <si>
     <t>UserName</t>
   </si>
@@ -163,36 +163,9 @@
     <t>110</t>
   </si>
   <si>
-    <t>0100</t>
-  </si>
-  <si>
-    <t>Automation WPR Project815339</t>
-  </si>
-  <si>
-    <t>101 Projects</t>
-  </si>
-  <si>
-    <t>Consultancies</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>16146 Merle Harbors</t>
-  </si>
-  <si>
-    <t>New Olinfurt</t>
-  </si>
-  <si>
-    <t>32547</t>
-  </si>
-  <si>
-    <t>WPR006168</t>
-  </si>
-  <si>
     <t>PhoneNo</t>
   </si>
   <si>
@@ -403,18 +376,12 @@
     <t>TeamEmailID</t>
   </si>
   <si>
-    <t>Automation V2 Project1632420</t>
-  </si>
-  <si>
     <t>Virgin Islands</t>
   </si>
   <si>
     <t>41512</t>
   </si>
   <si>
-    <t>2202266805</t>
-  </si>
-  <si>
     <t>101 Moorgate</t>
   </si>
   <si>
@@ -466,17 +433,22 @@
     <t>011977</t>
   </si>
   <si>
-    <t>WPR006261</t>
-  </si>
-  <si>
     <t>Automation V2 Project7886342</t>
+  </si>
+  <si>
+    <t>2202266808</t>
+  </si>
+  <si>
+    <t>gokulthiru22@gmail.com</t>
+  </si>
+  <si>
+    <t>WPR006273</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -812,10 +784,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -873,22 +845,22 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -899,16 +871,16 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -932,51 +904,51 @@
         <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="L2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="M2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="N2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -992,15 +964,15 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1020,39 +992,39 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -1068,39 +1040,38 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.21875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.21875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.21875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="4.44140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.88671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="5.44140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1130,7 +1101,7 @@
         <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="L1" t="s">
         <v>18</v>
@@ -1142,10 +1113,10 @@
         <v>9</v>
       </c>
       <c r="O1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="P1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="Q1" t="s">
         <v>29</v>
@@ -1163,69 +1134,69 @@
         <v>23</v>
       </c>
       <c r="V1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
       <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
         <v>124</v>
-      </c>
-      <c r="F2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" t="s">
-        <v>135</v>
       </c>
       <c r="I2" t="s">
         <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="L2" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="M2" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="N2" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="O2" t="s">
         <v>33</v>
       </c>
       <c r="P2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="Q2" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="R2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="S2" t="s">
         <v>35</v>
@@ -1237,7 +1208,10 @@
         <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+      <c r="X2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1254,20 +1228,20 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.21875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="30.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1275,7 +1249,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -1293,27 +1267,27 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -1322,28 +1296,28 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I2" t="s">
         <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1356,32 +1330,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F8409-99F8-4FFC-AA3A-80D15FF5718E}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="31.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.44140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="7.77734375" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -1402,7 +1376,7 @@
         <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K1" t="s">
         <v>16</v>
@@ -1410,13 +1384,13 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
@@ -1425,22 +1399,22 @@
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J2" t="s">
         <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1452,29 +1426,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6328ECB3-CDE0-459F-815E-F1AAB0123146}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.015625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.05859375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.11328125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.09375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.3828125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.0859375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.57421875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.44921875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.39453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.86328125" collapsed="true"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1486,7 +1460,7 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
@@ -1512,31 +1486,31 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="I2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -1545,7 +1519,7 @@
         <v>42</v>
       </c>
       <c r="L2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1561,32 +1535,32 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="4.44140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
@@ -1595,10 +1569,10 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
@@ -1609,34 +1583,34 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix for soft assert
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7DE833-2434-450A-B755-94E05F8CE02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F47B89-92D3-4CD7-8B1B-57AB5E3F354C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="204">
   <si>
     <t>UserName</t>
   </si>
@@ -142,9 +142,6 @@
     <t>100 RESILIENT CITIES</t>
   </si>
   <si>
-    <t>Manufacturing</t>
-  </si>
-  <si>
     <t>Montana</t>
   </si>
   <si>
@@ -172,18 +169,12 @@
     <t>APLanguage</t>
   </si>
   <si>
-    <t>Aerospace &amp; Aviation</t>
-  </si>
-  <si>
     <t>Delos</t>
   </si>
   <si>
     <t>English</t>
   </si>
   <si>
-    <t>w633305715c722</t>
-  </si>
-  <si>
     <t>WFEmp</t>
   </si>
   <si>
@@ -196,18 +187,6 @@
     <t>FullTime</t>
   </si>
   <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>06507 Marylynn Ford</t>
-  </si>
-  <si>
-    <t>DuBuqueborough</t>
-  </si>
-  <si>
-    <t>26329</t>
-  </si>
-  <si>
     <t>Organizationwebsite</t>
   </si>
   <si>
@@ -229,27 +208,9 @@
     <t>https://test-nuxt.wellcertified.com/</t>
   </si>
   <si>
-    <t>Lisbeth</t>
-  </si>
-  <si>
-    <t>Cedrick</t>
-  </si>
-  <si>
-    <t>dewey.brekke@yahoo.com</t>
-  </si>
-  <si>
-    <t>9702082995</t>
-  </si>
-  <si>
     <t>American Samoa</t>
   </si>
   <si>
-    <t>358 Gilberto Coves</t>
-  </si>
-  <si>
-    <t>Towneburgh</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -280,48 +241,9 @@
     <t>HsrName</t>
   </si>
   <si>
-    <t>HSRP006238</t>
-  </si>
-  <si>
-    <t>Automation HSR Project 7162135</t>
-  </si>
-  <si>
     <t>1-800 Flowers.com Inc.</t>
   </si>
   <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>074 Krystyna Shoal</t>
-  </si>
-  <si>
-    <t>Chantayburgh</t>
-  </si>
-  <si>
-    <t>00030-5564</t>
-  </si>
-  <si>
-    <t>015332</t>
-  </si>
-  <si>
-    <t>Norris</t>
-  </si>
-  <si>
-    <t>6935 Lizette Ridges</t>
-  </si>
-  <si>
-    <t>West Marinda</t>
-  </si>
-  <si>
-    <t>95210</t>
-  </si>
-  <si>
-    <t>1830104860</t>
-  </si>
-  <si>
-    <t>Wilburn</t>
-  </si>
-  <si>
     <t>OrgName</t>
   </si>
   <si>
@@ -334,163 +256,401 @@
     <t>TeamEmailID</t>
   </si>
   <si>
+    <t>ProjectID</t>
+  </si>
+  <si>
+    <t>gokulthiru22@gmail.com</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>CardCVC</t>
+  </si>
+  <si>
+    <t>CardExpDate</t>
+  </si>
+  <si>
+    <t>ProjectScope</t>
+  </si>
+  <si>
+    <t>ProjectGoals</t>
+  </si>
+  <si>
+    <t>BillingName</t>
+  </si>
+  <si>
+    <t>BillingOrganization</t>
+  </si>
+  <si>
+    <t>BillingStatus</t>
+  </si>
+  <si>
+    <t>ChallengeNote</t>
+  </si>
+  <si>
+    <t>CommunicationNote</t>
+  </si>
+  <si>
+    <t>BillingNote</t>
+  </si>
+  <si>
+    <t>ProjectScope Testing</t>
+  </si>
+  <si>
+    <t>ProjectGoals Testing</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>BillingOrganization Test</t>
+  </si>
+  <si>
+    <t>BillingStatus Test</t>
+  </si>
+  <si>
+    <t>ChallengeNote Test</t>
+  </si>
+  <si>
+    <t>CommunicationNote Test</t>
+  </si>
+  <si>
+    <t>BillingNote Test</t>
+  </si>
+  <si>
+    <t>Automation V2 Project7921697</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>43901</t>
+  </si>
+  <si>
+    <t>2202267602</t>
+  </si>
+  <si>
+    <t>Stacy</t>
+  </si>
+  <si>
+    <t>dominique.kessler@hotmail.com</t>
+  </si>
+  <si>
+    <t>5506461948</t>
+  </si>
+  <si>
+    <t>Materials &amp; Chemicals</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>74737 Franecki Underpass</t>
+  </si>
+  <si>
+    <t>Bergestad</t>
+  </si>
+  <si>
+    <t>61337</t>
+  </si>
+  <si>
+    <t>Lonny</t>
+  </si>
+  <si>
+    <t>Letter of Assurance – Engineer</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>08201 Rohan Glen</t>
+  </si>
+  <si>
+    <t>Wymanbury</t>
+  </si>
+  <si>
+    <t>48650</t>
+  </si>
+  <si>
+    <t>3332769997</t>
+  </si>
+  <si>
+    <t>Abe</t>
+  </si>
+  <si>
+    <t>Management Consulting</t>
+  </si>
+  <si>
+    <t>Nicol</t>
+  </si>
+  <si>
+    <t>w633e80d90291d</t>
+  </si>
+  <si>
+    <t>36055 Halvorson Alley</t>
+  </si>
+  <si>
+    <t>Henrystad</t>
+  </si>
+  <si>
+    <t>26973</t>
+  </si>
+  <si>
+    <t>Tajuana</t>
+  </si>
+  <si>
+    <t>Sidney</t>
+  </si>
+  <si>
+    <t>duncan.rau@hotmail.com</t>
+  </si>
+  <si>
+    <t>7711732876</t>
+  </si>
+  <si>
+    <t>7814 Josiah Turnpike</t>
+  </si>
+  <si>
+    <t>Wardport</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>Automation portfolio 3759932</t>
+  </si>
+  <si>
+    <t>Fitness &amp; Recreation</t>
+  </si>
+  <si>
+    <t>47084</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>585 Adrianna Port</t>
+  </si>
+  <si>
+    <t>East Cornelia</t>
+  </si>
+  <si>
+    <t>41621</t>
+  </si>
+  <si>
+    <t>WELLP06386</t>
+  </si>
+  <si>
+    <t>Delores</t>
+  </si>
+  <si>
+    <t>concha.simonis@gmail.com</t>
+  </si>
+  <si>
+    <t>1846144814</t>
+  </si>
+  <si>
+    <t>Jeffery</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>046 Dorian Key</t>
+  </si>
+  <si>
+    <t>Bauchview</t>
+  </si>
+  <si>
+    <t>63126-2316</t>
+  </si>
+  <si>
+    <t>5700</t>
+  </si>
+  <si>
+    <t>Bok</t>
+  </si>
+  <si>
+    <t>HSRP006387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation HSR Project </t>
+  </si>
+  <si>
+    <t>Automation WPR Project2348355</t>
+  </si>
+  <si>
+    <t>Education Support</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>25892 Fahey Fords</t>
+  </si>
+  <si>
+    <t>Charleyfurt</t>
+  </si>
+  <si>
+    <t>65896</t>
+  </si>
+  <si>
+    <t>025023</t>
+  </si>
+  <si>
+    <t>Alvaro</t>
+  </si>
+  <si>
+    <t>WPR006388</t>
+  </si>
+  <si>
+    <t>Automation WPR Project6336645</t>
+  </si>
+  <si>
     <t>101 Moorgate</t>
   </si>
   <si>
-    <t>Linette</t>
-  </si>
-  <si>
-    <t>ashley.jacobs@gmail.com</t>
-  </si>
-  <si>
-    <t>4688505956</t>
-  </si>
-  <si>
-    <t>Medical Support</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>ProjectID</t>
-  </si>
-  <si>
-    <t>Automation WPR Project1839088</t>
-  </si>
-  <si>
-    <t>Building Services</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>06524 Rowena Ports</t>
-  </si>
-  <si>
-    <t>Lake Ione</t>
-  </si>
-  <si>
-    <t>38923-0738</t>
-  </si>
-  <si>
-    <t>011977</t>
-  </si>
-  <si>
-    <t>gokulthiru22@gmail.com</t>
-  </si>
-  <si>
-    <t>WPR006273</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>CardCVC</t>
-  </si>
-  <si>
-    <t>CardExpDate</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>16095</t>
-  </si>
-  <si>
-    <t>Automation V2 Project6045912</t>
-  </si>
-  <si>
-    <t>2202266982</t>
-  </si>
-  <si>
-    <t>Automation portfolio 5698076</t>
-  </si>
-  <si>
-    <t>Education Support</t>
-  </si>
-  <si>
-    <t>8108</t>
-  </si>
-  <si>
-    <t>108 Watsica Knolls</t>
-  </si>
-  <si>
-    <t>South Eltonchester</t>
-  </si>
-  <si>
-    <t>07007</t>
-  </si>
-  <si>
-    <t>WELLP06306</t>
-  </si>
-  <si>
-    <t>Christiane</t>
-  </si>
-  <si>
-    <t>stephan.conn@gmail.com</t>
-  </si>
-  <si>
-    <t>8077847477</t>
-  </si>
-  <si>
-    <t>Priscilla</t>
-  </si>
-  <si>
-    <t>ProjectScope</t>
-  </si>
-  <si>
-    <t>ProjectGoals</t>
-  </si>
-  <si>
-    <t>BillingName</t>
-  </si>
-  <si>
-    <t>BillingOrganization</t>
-  </si>
-  <si>
-    <t>BillingStatus</t>
-  </si>
-  <si>
-    <t>ChallengeNote</t>
-  </si>
-  <si>
-    <t>CommunicationNote</t>
-  </si>
-  <si>
-    <t>BillingNote</t>
-  </si>
-  <si>
-    <t>ProjectScope Testing</t>
-  </si>
-  <si>
-    <t>ProjectGoals Testing</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>BillingOrganization Test</t>
-  </si>
-  <si>
-    <t>BillingStatus Test</t>
-  </si>
-  <si>
-    <t>ChallengeNote Test</t>
-  </si>
-  <si>
-    <t>CommunicationNote Test</t>
-  </si>
-  <si>
-    <t>BillingNote Test</t>
+    <t>Air Travel</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>460 Herschel Via</t>
+  </si>
+  <si>
+    <t>East Justin</t>
+  </si>
+  <si>
+    <t>83289-0351</t>
+  </si>
+  <si>
+    <t>03489</t>
+  </si>
+  <si>
+    <t>Myron</t>
+  </si>
+  <si>
+    <t>WPR006389</t>
+  </si>
+  <si>
+    <t>Automation WPR Project4740366</t>
+  </si>
+  <si>
+    <t>Retirement Communities</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>22638 Lueilwitz Mountains</t>
+  </si>
+  <si>
+    <t>Margertburgh</t>
+  </si>
+  <si>
+    <t>42923</t>
+  </si>
+  <si>
+    <t>25236</t>
+  </si>
+  <si>
+    <t>Maximo</t>
+  </si>
+  <si>
+    <t>WPR006390</t>
+  </si>
+  <si>
+    <t>Automation WPR Project1777385</t>
+  </si>
+  <si>
+    <t>Warehousing &amp; Storage</t>
+  </si>
+  <si>
+    <t>22245 Spencer Ford</t>
+  </si>
+  <si>
+    <t>Lake Clarissaview</t>
+  </si>
+  <si>
+    <t>47942-9097</t>
+  </si>
+  <si>
+    <t>38518</t>
+  </si>
+  <si>
+    <t>Shayne</t>
+  </si>
+  <si>
+    <t>WPR006391</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 3959142</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 5227661</t>
+  </si>
+  <si>
+    <t>Post Secondary Education</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>9679 Windler Points</t>
+  </si>
+  <si>
+    <t>East Wava</t>
+  </si>
+  <si>
+    <t>71218-4286</t>
+  </si>
+  <si>
+    <t>2289</t>
+  </si>
+  <si>
+    <t>Trina</t>
+  </si>
+  <si>
+    <t>HSRP006392</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 7224818</t>
+  </si>
+  <si>
+    <t>Oil &amp; Gas</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>68558 Boyer Crest</t>
+  </si>
+  <si>
+    <t>North Huefurt</t>
+  </si>
+  <si>
+    <t>97551</t>
+  </si>
+  <si>
+    <t>9132</t>
+  </si>
+  <si>
+    <t>Amos</t>
+  </si>
+  <si>
+    <t>HSRP006393</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -534,13 +694,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -830,8 +989,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -891,30 +1050,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="10" max="11" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -923,16 +1081,16 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
@@ -956,69 +1114,69 @@
         <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="P1" t="s">
         <v>20</v>
       </c>
       <c r="Q1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="R1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="S1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
         <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>126</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="J2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="O2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="P2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="Q2" t="s">
         <v>32</v>
@@ -1045,13 +1203,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1071,39 +1230,39 @@
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -1118,40 +1277,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DDA08-C4FB-4E43-ADE7-EDDAA41E68CF}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="63.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="21" max="22" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1181,7 +1340,7 @@
         <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="L1" t="s">
         <v>18</v>
@@ -1193,10 +1352,10 @@
         <v>9</v>
       </c>
       <c r="O1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="P1" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="Q1" t="s">
         <v>26</v>
@@ -1205,102 +1364,102 @@
         <v>20</v>
       </c>
       <c r="S1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="T1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="U1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="V1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="W1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" t="s">
         <v>79</v>
       </c>
-      <c r="X1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>142</v>
+      <c r="Z1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="4" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="I2" t="s">
         <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="K2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" t="s">
         <v>100</v>
       </c>
-      <c r="L2" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>102</v>
-      </c>
-      <c r="N2" t="s">
-        <v>104</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R2" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="S2" t="s">
         <v>32</v>
@@ -1312,37 +1471,37 @@
         <v>34</v>
       </c>
       <c r="V2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="W2" t="s">
         <v>13</v>
       </c>
       <c r="X2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>150</v>
+        <v>75</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1361,22 +1520,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1384,7 +1543,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -1402,72 +1561,72 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
-      </c>
-      <c r="L1" t="s">
-        <v>45</v>
       </c>
       <c r="M1" t="s">
         <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="O1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="P1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" t="s">
         <v>46</v>
       </c>
-      <c r="K2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
       <c r="M2" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="N2" t="s">
         <v>32</v>
@@ -1489,38 +1648,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F8409-99F8-4FFC-AA3A-80D15FF5718E}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="30.95703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.62109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.1875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.3203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="5.49609375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -1541,7 +1700,7 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="K1" t="s">
         <v>16</v>
@@ -1550,51 +1709,51 @@
         <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="N1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>196</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>198</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
       <c r="I2" t="s">
-        <v>88</v>
+        <v>200</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="L2" t="s">
-        <v>90</v>
+        <v>202</v>
       </c>
       <c r="M2" t="s">
         <v>32</v>
@@ -1615,33 +1774,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6328ECB3-CDE0-459F-815E-F1AAB0123146}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.015625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.171875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.1328125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.76953125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.53515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.64453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.44921875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.39453125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.86328125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1653,7 +1812,7 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
@@ -1680,54 +1839,54 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="O1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="P1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="G2" t="s">
-        <v>110</v>
+        <v>179</v>
       </c>
       <c r="H2" t="s">
-        <v>111</v>
+        <v>180</v>
       </c>
       <c r="I2" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" t="s">
-        <v>39</v>
-      </c>
       <c r="L2" t="s">
-        <v>113</v>
+        <v>182</v>
       </c>
       <c r="M2" t="s">
-        <v>90</v>
+        <v>183</v>
       </c>
       <c r="N2" t="s">
         <v>32</v>
@@ -1754,34 +1913,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
@@ -1790,10 +1949,10 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
         <v>22</v>
@@ -1805,48 +1964,48 @@
         <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="M1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="N1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="K2" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
       <c r="L2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
TestNg file modifying and Test method creation
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F47B89-92D3-4CD7-8B1B-57AB5E3F354C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430F0CBD-A812-4402-99DB-308D21AFD8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="163">
   <si>
     <t>UserName</t>
   </si>
@@ -139,9 +139,6 @@
     <t>999</t>
   </si>
   <si>
-    <t>100 RESILIENT CITIES</t>
-  </si>
-  <si>
     <t>Montana</t>
   </si>
   <si>
@@ -319,48 +316,9 @@
     <t>BillingNote Test</t>
   </si>
   <si>
-    <t>Automation V2 Project7921697</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>43901</t>
-  </si>
-  <si>
-    <t>2202267602</t>
-  </si>
-  <si>
-    <t>Stacy</t>
-  </si>
-  <si>
-    <t>dominique.kessler@hotmail.com</t>
-  </si>
-  <si>
-    <t>5506461948</t>
-  </si>
-  <si>
-    <t>Materials &amp; Chemicals</t>
-  </si>
-  <si>
     <t>Wyoming</t>
   </si>
   <si>
-    <t>74737 Franecki Underpass</t>
-  </si>
-  <si>
-    <t>Bergestad</t>
-  </si>
-  <si>
-    <t>61337</t>
-  </si>
-  <si>
-    <t>Lonny</t>
-  </si>
-  <si>
-    <t>Letter of Assurance – Engineer</t>
-  </si>
-  <si>
     <t>Utah</t>
   </si>
   <si>
@@ -454,117 +412,12 @@
     <t>Jeffery</t>
   </si>
   <si>
-    <t>Community</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>046 Dorian Key</t>
-  </si>
-  <si>
-    <t>Bauchview</t>
-  </si>
-  <si>
-    <t>63126-2316</t>
-  </si>
-  <si>
-    <t>5700</t>
-  </si>
-  <si>
-    <t>Bok</t>
-  </si>
-  <si>
-    <t>HSRP006387</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation HSR Project </t>
-  </si>
-  <si>
-    <t>Automation WPR Project2348355</t>
-  </si>
-  <si>
-    <t>Education Support</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>25892 Fahey Fords</t>
-  </si>
-  <si>
-    <t>Charleyfurt</t>
-  </si>
-  <si>
-    <t>65896</t>
-  </si>
-  <si>
-    <t>025023</t>
-  </si>
-  <si>
-    <t>Alvaro</t>
-  </si>
-  <si>
-    <t>WPR006388</t>
-  </si>
-  <si>
-    <t>Automation WPR Project6336645</t>
-  </si>
-  <si>
     <t>101 Moorgate</t>
   </si>
   <si>
     <t>Air Travel</t>
   </si>
   <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>460 Herschel Via</t>
-  </si>
-  <si>
-    <t>East Justin</t>
-  </si>
-  <si>
-    <t>83289-0351</t>
-  </si>
-  <si>
-    <t>03489</t>
-  </si>
-  <si>
-    <t>Myron</t>
-  </si>
-  <si>
-    <t>WPR006389</t>
-  </si>
-  <si>
-    <t>Automation WPR Project4740366</t>
-  </si>
-  <si>
-    <t>Retirement Communities</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>22638 Lueilwitz Mountains</t>
-  </si>
-  <si>
-    <t>Margertburgh</t>
-  </si>
-  <si>
-    <t>42923</t>
-  </si>
-  <si>
-    <t>25236</t>
-  </si>
-  <si>
-    <t>Maximo</t>
-  </si>
-  <si>
-    <t>WPR006390</t>
-  </si>
-  <si>
     <t>Automation WPR Project1777385</t>
   </si>
   <si>
@@ -589,36 +442,6 @@
     <t>WPR006391</t>
   </si>
   <si>
-    <t>Automation HSR Project 3959142</t>
-  </si>
-  <si>
-    <t>Automation HSR Project 5227661</t>
-  </si>
-  <si>
-    <t>Post Secondary Education</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>9679 Windler Points</t>
-  </si>
-  <si>
-    <t>East Wava</t>
-  </si>
-  <si>
-    <t>71218-4286</t>
-  </si>
-  <si>
-    <t>2289</t>
-  </si>
-  <si>
-    <t>Trina</t>
-  </si>
-  <si>
-    <t>HSRP006392</t>
-  </si>
-  <si>
     <t>Automation HSR Project 7224818</t>
   </si>
   <si>
@@ -644,6 +467,60 @@
   </si>
   <si>
     <t>HSRP006393</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Maegan</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Irina</t>
+  </si>
+  <si>
+    <t>Automation V2 Project2475539</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>43253</t>
+  </si>
+  <si>
+    <t>2202267753</t>
+  </si>
+  <si>
+    <t>Ernie</t>
+  </si>
+  <si>
+    <t>cammy.brakus@hotmail.com</t>
+  </si>
+  <si>
+    <t>5231167562</t>
+  </si>
+  <si>
+    <t>Automation V2 Project4484667</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>9522 Rempel Hollow</t>
+  </si>
+  <si>
+    <t>Russelside</t>
+  </si>
+  <si>
+    <t>39006-5051</t>
+  </si>
+  <si>
+    <t>20252</t>
+  </si>
+  <si>
+    <t>2202267755</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +949,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -1081,16 +958,16 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>60</v>
-      </c>
-      <c r="G1" t="s">
-        <v>61</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
@@ -1114,69 +991,69 @@
         <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P1" t="s">
         <v>20</v>
       </c>
       <c r="Q1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" t="s">
         <v>76</v>
-      </c>
-      <c r="R1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="K2" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="L2" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="M2" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="N2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="O2" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="P2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="Q2" t="s">
         <v>32</v>
@@ -1230,39 +1107,39 @@
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
       <c r="I1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -1277,30 +1154,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DDA08-C4FB-4E43-ADE7-EDDAA41E68CF}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="63.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.12890625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.4765625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="4.44921875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="14" max="15" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="21" max="22" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
@@ -1310,7 +1186,7 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1340,7 +1216,7 @@
         <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
         <v>18</v>
@@ -1352,10 +1228,10 @@
         <v>9</v>
       </c>
       <c r="O1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" t="s">
         <v>71</v>
-      </c>
-      <c r="P1" t="s">
-        <v>72</v>
       </c>
       <c r="Q1" t="s">
         <v>26</v>
@@ -1364,102 +1240,102 @@
         <v>20</v>
       </c>
       <c r="S1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" t="s">
         <v>78</v>
       </c>
-      <c r="U1" t="s">
-        <v>77</v>
-      </c>
-      <c r="V1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W1" t="s">
-        <v>66</v>
-      </c>
-      <c r="X1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>80</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>81</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>82</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>84</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>85</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>158</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="I2" t="s">
         <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="K2" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="M2" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="N2" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="Q2" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="R2" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
       <c r="S2" t="s">
         <v>32</v>
@@ -1471,37 +1347,37 @@
         <v>34</v>
       </c>
       <c r="V2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W2" t="s">
         <v>13</v>
       </c>
       <c r="X2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z2" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>88</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>89</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>90</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>91</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>92</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>93</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1543,7 +1419,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -1561,72 +1437,72 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>44</v>
       </c>
       <c r="M1" t="s">
         <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" t="s">
         <v>76</v>
-      </c>
-      <c r="O1" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="K2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" t="s">
         <v>45</v>
       </c>
-      <c r="L2" t="s">
-        <v>46</v>
-      </c>
       <c r="M2" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="N2" t="s">
         <v>32</v>
@@ -1654,18 +1530,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="30.95703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.62109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.1875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.3203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="5.49609375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="31.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
@@ -1673,13 +1549,13 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -1700,7 +1576,7 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
         <v>16</v>
@@ -1709,51 +1585,51 @@
         <v>20</v>
       </c>
       <c r="M1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" t="s">
         <v>76</v>
-      </c>
-      <c r="N1" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
-        <v>203</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>138</v>
       </c>
       <c r="G2" t="s">
-        <v>198</v>
+        <v>139</v>
       </c>
       <c r="H2" t="s">
-        <v>199</v>
+        <v>140</v>
       </c>
       <c r="I2" t="s">
-        <v>200</v>
+        <v>141</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="L2" t="s">
-        <v>202</v>
+        <v>143</v>
       </c>
       <c r="M2" t="s">
         <v>32</v>
@@ -1774,25 +1650,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6328ECB3-CDE0-459F-815E-F1AAB0123146}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.015625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.171875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.1328125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.76953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.53515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.64453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.44921875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.39453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.86328125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
@@ -1800,7 +1676,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1812,7 +1688,7 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
@@ -1839,54 +1715,54 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" t="s">
         <v>76</v>
-      </c>
-      <c r="O1" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="I2" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s">
-        <v>38</v>
-      </c>
       <c r="L2" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="M2" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="N2" t="s">
         <v>32</v>
@@ -1931,16 +1807,16 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
@@ -1949,10 +1825,10 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
         <v>22</v>
@@ -1964,48 +1840,48 @@
         <v>20</v>
       </c>
       <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" t="s">
         <v>76</v>
-      </c>
-      <c r="M1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="J2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Combined TestNg file modification
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="211">
   <si>
     <t>UserName</t>
   </si>
@@ -521,6 +521,150 @@
   </si>
   <si>
     <t>2202267755</t>
+  </si>
+  <si>
+    <t>Automation V2 Project203564</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>037 Silas Walks</t>
+  </si>
+  <si>
+    <t>South Virgilio</t>
+  </si>
+  <si>
+    <t>70017</t>
+  </si>
+  <si>
+    <t>39601</t>
+  </si>
+  <si>
+    <t>2202268159</t>
+  </si>
+  <si>
+    <t>Kiesha</t>
+  </si>
+  <si>
+    <t>carin.dare@yahoo.com</t>
+  </si>
+  <si>
+    <t>3934935862</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Northern Mariana Isl</t>
+  </si>
+  <si>
+    <t>974 Ward Highway</t>
+  </si>
+  <si>
+    <t>Luettgenbury</t>
+  </si>
+  <si>
+    <t>87448</t>
+  </si>
+  <si>
+    <t>Terrance</t>
+  </si>
+  <si>
+    <t>Policy and/or Operations Schedule</t>
+  </si>
+  <si>
+    <t>Automation V2 Project3636887</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>8268 Andreas Villages</t>
+  </si>
+  <si>
+    <t>Loweshire</t>
+  </si>
+  <si>
+    <t>89723</t>
+  </si>
+  <si>
+    <t>17025</t>
+  </si>
+  <si>
+    <t>2202268177</t>
+  </si>
+  <si>
+    <t>Ronny</t>
+  </si>
+  <si>
+    <t>tory.kautzer@gmail.com</t>
+  </si>
+  <si>
+    <t>1145131349</t>
+  </si>
+  <si>
+    <t>Early Childcare</t>
+  </si>
+  <si>
+    <t>952 Soledad Mills</t>
+  </si>
+  <si>
+    <t>East Rosalynborough</t>
+  </si>
+  <si>
+    <t>47586-9537</t>
+  </si>
+  <si>
+    <t>Alec</t>
+  </si>
+  <si>
+    <t>Automation V2 Project1572821</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>144 Beatris Rest</t>
+  </si>
+  <si>
+    <t>Tylermouth</t>
+  </si>
+  <si>
+    <t>43346</t>
+  </si>
+  <si>
+    <t>14365</t>
+  </si>
+  <si>
+    <t>2202268178</t>
+  </si>
+  <si>
+    <t>Alleen</t>
+  </si>
+  <si>
+    <t>forest.maggio@gmail.com</t>
+  </si>
+  <si>
+    <t>8905606588</t>
+  </si>
+  <si>
+    <t>Wellness Services</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>80237 Fiona Spurs</t>
+  </si>
+  <si>
+    <t>Halvorsonburgh</t>
+  </si>
+  <si>
+    <t>52672</t>
+  </si>
+  <si>
+    <t>Cheyenne</t>
   </si>
 </sst>
 </file>
@@ -1162,26 +1306,28 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.12890625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.4765625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="4.44921875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.8125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.4765625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.4375" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.921875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="14" max="15" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.734375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.15625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.23046875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.8125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="21" max="22" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.51171875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.6484375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="23.671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -1284,58 +1430,58 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="4" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>196</v>
       </c>
       <c r="F2" t="s">
-        <v>158</v>
+        <v>207</v>
       </c>
       <c r="G2" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="I2" t="s">
         <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="L2" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="M2" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="N2" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="Q2" t="s">
-        <v>146</v>
+        <v>202</v>
       </c>
       <c r="R2" t="s">
-        <v>148</v>
+        <v>210</v>
       </c>
       <c r="S2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Facutlty Testng file modification
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="244">
   <si>
     <t>UserName</t>
   </si>
@@ -755,6 +755,15 @@
   </si>
   <si>
     <t>2202268737</t>
+  </si>
+  <si>
+    <t>7244 Rau Station</t>
+  </si>
+  <si>
+    <t>Russton</t>
+  </si>
+  <si>
+    <t>65762-0220</t>
   </si>
 </sst>
 </file>
@@ -1322,14 +1331,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.74609375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7890625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.64453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.71875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1366,16 +1375,16 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
fix for Custom Scorecard
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="443">
   <si>
     <t>UserName</t>
   </si>
@@ -1227,6 +1227,141 @@
   </si>
   <si>
     <t>13519-1518</t>
+  </si>
+  <si>
+    <t>Automation portfolio 3386090</t>
+  </si>
+  <si>
+    <t>46768</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>97348 Waters Hill</t>
+  </si>
+  <si>
+    <t>Jenellland</t>
+  </si>
+  <si>
+    <t>17304-1646</t>
+  </si>
+  <si>
+    <t>WELLP07133</t>
+  </si>
+  <si>
+    <t>Kenia</t>
+  </si>
+  <si>
+    <t>karri.gleichner@hotmail.com</t>
+  </si>
+  <si>
+    <t>0206552567</t>
+  </si>
+  <si>
+    <t>Tynisha</t>
+  </si>
+  <si>
+    <t>Automation portfolio 2538556</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>40313</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>400 Garry Course</t>
+  </si>
+  <si>
+    <t>Mohrtown</t>
+  </si>
+  <si>
+    <t>61642-3111</t>
+  </si>
+  <si>
+    <t>WELLP07134</t>
+  </si>
+  <si>
+    <t>Vern</t>
+  </si>
+  <si>
+    <t>felisa.crist@hotmail.com</t>
+  </si>
+  <si>
+    <t>2808075671</t>
+  </si>
+  <si>
+    <t>Giuseppe</t>
+  </si>
+  <si>
+    <t>Automation portfolio 2343247</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>35226</t>
+  </si>
+  <si>
+    <t>82753 Sandy Prairie</t>
+  </si>
+  <si>
+    <t>Lake Santos</t>
+  </si>
+  <si>
+    <t>60876</t>
+  </si>
+  <si>
+    <t>WELLP07136</t>
+  </si>
+  <si>
+    <t>Herb</t>
+  </si>
+  <si>
+    <t>rosalyn.gaylord@gmail.com</t>
+  </si>
+  <si>
+    <t>8971038170</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>Automation portfolio 1695885</t>
+  </si>
+  <si>
+    <t>36706</t>
+  </si>
+  <si>
+    <t>Virgin Islands</t>
+  </si>
+  <si>
+    <t>02266 Darci Ramp</t>
+  </si>
+  <si>
+    <t>Shermanland</t>
+  </si>
+  <si>
+    <t>38555-1839</t>
+  </si>
+  <si>
+    <t>WELLP07137</t>
+  </si>
+  <si>
+    <t>Vance</t>
+  </si>
+  <si>
+    <t>millard.huels@hotmail.com</t>
+  </si>
+  <si>
+    <t>4411720046</t>
+  </si>
+  <si>
+    <t>Ulysses</t>
   </si>
 </sst>
 </file>
@@ -2103,18 +2238,18 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.62890625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.82421875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.6796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="27.1171875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="9.80078125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.78515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.609375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.69140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.9609375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.80859375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.5859375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.66015625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="25.9921875" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
@@ -2225,16 +2360,16 @@
     </row>
     <row r="2" spans="1:30" ht="30">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>438</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>432</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>277</v>
       </c>
       <c r="E2" t="s">
         <v>60</v>
@@ -2243,34 +2378,34 @@
         <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>316</v>
+        <v>433</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>146</v>
+        <v>434</v>
       </c>
       <c r="J2" t="s">
-        <v>317</v>
+        <v>435</v>
       </c>
       <c r="K2" t="s">
-        <v>318</v>
+        <v>436</v>
       </c>
       <c r="L2" t="s">
-        <v>319</v>
+        <v>437</v>
       </c>
       <c r="M2" t="s">
-        <v>321</v>
+        <v>439</v>
       </c>
       <c r="N2" t="s">
-        <v>322</v>
+        <v>440</v>
       </c>
       <c r="O2" t="s">
-        <v>323</v>
+        <v>441</v>
       </c>
       <c r="P2" t="s">
-        <v>324</v>
+        <v>442</v>
       </c>
       <c r="Q2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
added code for membership
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF30FBA-53F6-4B03-ACA1-D6B7302FDF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E54B432-DBCB-4B3F-9626-D99BDFE8992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="260">
   <si>
     <t>UserName</t>
   </si>
@@ -137,9 +137,6 @@
     <t>999</t>
   </si>
   <si>
-    <t>Montana</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -389,15 +386,6 @@
     <t>OwnerPostalCode</t>
   </si>
   <si>
-    <t>7244 Rau Station</t>
-  </si>
-  <si>
-    <t>Russton</t>
-  </si>
-  <si>
-    <t>65762-0220</t>
-  </si>
-  <si>
     <t>Jimmie</t>
   </si>
   <si>
@@ -434,36 +422,12 @@
     <t>Alaska</t>
   </si>
   <si>
-    <t>Jazmin</t>
-  </si>
-  <si>
-    <t>Clayton</t>
-  </si>
-  <si>
-    <t>ron.feil@hotmail.com</t>
-  </si>
-  <si>
-    <t>0345911466</t>
-  </si>
-  <si>
-    <t>07299 Wilton Forge</t>
-  </si>
-  <si>
-    <t>Lake Vanesa</t>
-  </si>
-  <si>
-    <t>Merlin</t>
-  </si>
-  <si>
     <t>abhishek.gupta@wellcertified.com</t>
   </si>
   <si>
     <t>100 RESILIENT CITIES</t>
   </si>
   <si>
-    <t>Air Travel</t>
-  </si>
-  <si>
     <t>NoPurseCount</t>
   </si>
   <si>
@@ -473,9 +437,6 @@
     <t>ScorecardPartCount</t>
   </si>
   <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
     <t>4225</t>
   </si>
   <si>
@@ -521,9 +482,6 @@
     <t>Account notes testing</t>
   </si>
   <si>
-    <t>Melanie (melanie.koch@wellcertified.com)</t>
-  </si>
-  <si>
     <t>WELL Performance Rating scope &amp; premises</t>
   </si>
   <si>
@@ -578,57 +536,6 @@
     <t>75,750.00</t>
   </si>
   <si>
-    <t>Jerry</t>
-  </si>
-  <si>
-    <t>georgina.herman@hotmail.com</t>
-  </si>
-  <si>
-    <t>8344827387</t>
-  </si>
-  <si>
-    <t>204 Gino Knolls</t>
-  </si>
-  <si>
-    <t>Hermanshire</t>
-  </si>
-  <si>
-    <t>47108</t>
-  </si>
-  <si>
-    <t>Blake</t>
-  </si>
-  <si>
-    <t>Automation HSR Project 3183235</t>
-  </si>
-  <si>
-    <t>Retirement Communities</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>7050 Napoleon Pines</t>
-  </si>
-  <si>
-    <t>Murraytown</t>
-  </si>
-  <si>
-    <t>93233-2983</t>
-  </si>
-  <si>
-    <t>20562</t>
-  </si>
-  <si>
-    <t>Elvin</t>
-  </si>
-  <si>
-    <t>HSRP007045</t>
-  </si>
-  <si>
-    <t>2202272380</t>
-  </si>
-  <si>
     <t>Sabrina Stanger (sabrina.stanger@wellcertified.com)</t>
   </si>
   <si>
@@ -638,486 +545,24 @@
     <t>Paige (pmcknight@gbci.org)</t>
   </si>
   <si>
-    <t>Automation WPR Project7473173</t>
-  </si>
-  <si>
-    <t>101 Moorgate</t>
-  </si>
-  <si>
-    <t>Warehousing &amp; Storage</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>318 Willard Grove</t>
-  </si>
-  <si>
-    <t>New Miesha</t>
-  </si>
-  <si>
-    <t>50181-0544</t>
-  </si>
-  <si>
-    <t>7502</t>
-  </si>
-  <si>
-    <t>WPR007052</t>
-  </si>
-  <si>
-    <t>Automation V2 Project2709566</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>781 Stiedemann Lane</t>
-  </si>
-  <si>
-    <t>Lake Rossbury</t>
-  </si>
-  <si>
-    <t>35401</t>
-  </si>
-  <si>
-    <t>51379</t>
-  </si>
-  <si>
-    <t>Automation V2 Project485969</t>
-  </si>
-  <si>
-    <t>Zhejiang</t>
-  </si>
-  <si>
-    <t>87848 Renner Meadows</t>
-  </si>
-  <si>
-    <t>Hesselhaven</t>
-  </si>
-  <si>
-    <t>02714-3603</t>
-  </si>
-  <si>
-    <t>46616</t>
-  </si>
-  <si>
-    <t>2202272413</t>
-  </si>
-  <si>
-    <t>Automation portfolio 3884630</t>
-  </si>
-  <si>
-    <t>Media, PR &amp; Communications</t>
-  </si>
-  <si>
-    <t>10720</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>53427 Schaden Knoll</t>
-  </si>
-  <si>
-    <t>Port Nelson</t>
-  </si>
-  <si>
-    <t>73220-7408</t>
-  </si>
-  <si>
-    <t>WELLP07058</t>
-  </si>
-  <si>
-    <t>Renee</t>
-  </si>
-  <si>
-    <t>vicky.gleason@yahoo.com</t>
-  </si>
-  <si>
-    <t>5612407269</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
-    <t>Office Spaces</t>
-  </si>
-  <si>
     <t>$ 30,000.00 USD</t>
   </si>
   <si>
-    <t>Automation portfolio 1221855</t>
-  </si>
-  <si>
-    <t>Consultancies</t>
-  </si>
-  <si>
-    <t>36481</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>9736 Windler Cliffs</t>
-  </si>
-  <si>
-    <t>Leandrohaven</t>
-  </si>
-  <si>
-    <t>15501-4162</t>
-  </si>
-  <si>
-    <t>WELLP07059</t>
-  </si>
-  <si>
-    <t>Nikita</t>
-  </si>
-  <si>
-    <t>santa.marquardt@hotmail.com</t>
-  </si>
-  <si>
-    <t>1832377825</t>
-  </si>
-  <si>
-    <t>Kim</t>
-  </si>
-  <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
     <t>For sale/lease</t>
   </si>
   <si>
-    <t>Automation portfolio 5489308</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>33362</t>
-  </si>
-  <si>
     <t>Louisiana</t>
   </si>
   <si>
-    <t>354 Delena Garden</t>
-  </si>
-  <si>
-    <t>East Garrettborough</t>
-  </si>
-  <si>
-    <t>29463</t>
-  </si>
-  <si>
-    <t>WELLP07060</t>
-  </si>
-  <si>
-    <t>Zenaida</t>
-  </si>
-  <si>
-    <t>carrol.langosh@hotmail.com</t>
-  </si>
-  <si>
-    <t>8160068437</t>
-  </si>
-  <si>
-    <t>Wen</t>
-  </si>
-  <si>
-    <t>Automation portfolio 5042514</t>
-  </si>
-  <si>
-    <t>Construction</t>
-  </si>
-  <si>
-    <t>17076</t>
-  </si>
-  <si>
-    <t>900 Yost Parkway</t>
-  </si>
-  <si>
-    <t>Johnsmouth</t>
-  </si>
-  <si>
-    <t>34720-3258</t>
-  </si>
-  <si>
-    <t>Automation portfolio 3926920</t>
-  </si>
-  <si>
-    <t>Clinical Services</t>
-  </si>
-  <si>
-    <t>49391</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>02909 Tom Island</t>
-  </si>
-  <si>
-    <t>Tyronehaven</t>
-  </si>
-  <si>
-    <t>96873</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1279520</t>
-  </si>
-  <si>
     <t>100 Percent Group Limited</t>
   </si>
   <si>
-    <t>Manufacturing</t>
-  </si>
-  <si>
-    <t>14012</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>99964 Miguel Falls</t>
-  </si>
-  <si>
-    <t>Lake Noble</t>
-  </si>
-  <si>
-    <t>04997-0432</t>
-  </si>
-  <si>
-    <t>WELLP07066</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>hector.hagenes@hotmail.com</t>
-  </si>
-  <si>
-    <t>1387408551</t>
-  </si>
-  <si>
-    <t>Nichole</t>
-  </si>
-  <si>
-    <t>Convention Centers</t>
-  </si>
-  <si>
-    <t>Automation portfolio 6795991</t>
-  </si>
-  <si>
-    <t>21892</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>67180 Lillian Springs</t>
-  </si>
-  <si>
-    <t>Port Peter</t>
-  </si>
-  <si>
-    <t>40357</t>
-  </si>
-  <si>
-    <t>WELLP07067</t>
-  </si>
-  <si>
-    <t>Denna</t>
-  </si>
-  <si>
-    <t>alexia.padberg@gmail.com</t>
-  </si>
-  <si>
-    <t>6765048252</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Fitness</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1211367</t>
-  </si>
-  <si>
-    <t>Student Housing</t>
-  </si>
-  <si>
-    <t>34124</t>
-  </si>
-  <si>
-    <t>1526 Dusty Lock</t>
-  </si>
-  <si>
-    <t>Lake Carey</t>
-  </si>
-  <si>
-    <t>66340-2076</t>
-  </si>
-  <si>
-    <t>WELLP07068</t>
-  </si>
-  <si>
-    <t>Markus</t>
-  </si>
-  <si>
-    <t>robbie.jacobson@gmail.com</t>
-  </si>
-  <si>
-    <t>0203420649</t>
-  </si>
-  <si>
-    <t>Collene</t>
-  </si>
-  <si>
-    <t>Industrial</t>
-  </si>
-  <si>
-    <t>Mona (mona.holtkoetter@wellcertified.com)</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2695810</t>
-  </si>
-  <si>
-    <t>17841</t>
-  </si>
-  <si>
-    <t>759 Kovacek Plaza</t>
-  </si>
-  <si>
-    <t>Adalbertoville</t>
-  </si>
-  <si>
-    <t>40117</t>
-  </si>
-  <si>
-    <t>WELLP07069</t>
-  </si>
-  <si>
-    <t>Trevor</t>
-  </si>
-  <si>
-    <t>doris.okon@yahoo.com</t>
-  </si>
-  <si>
-    <t>3866554759</t>
-  </si>
-  <si>
-    <t>Lucio</t>
-  </si>
-  <si>
-    <t>Dwelling Units</t>
-  </si>
-  <si>
     <t>Karen (karen.quintana@wellcertified.com)</t>
   </si>
   <si>
-    <t>Automation V2 Project4388469</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>572 Lubowitz Cove</t>
-  </si>
-  <si>
-    <t>Lehnertown</t>
-  </si>
-  <si>
-    <t>56886-3973</t>
-  </si>
-  <si>
-    <t>53721</t>
-  </si>
-  <si>
-    <t>2202272598</t>
-  </si>
-  <si>
-    <t>Automation V2 Project3222142</t>
-  </si>
-  <si>
-    <t>Ningxia</t>
-  </si>
-  <si>
-    <t>0733 Abernathy Common</t>
-  </si>
-  <si>
-    <t>South Edmundo</t>
-  </si>
-  <si>
-    <t>90523-8146</t>
-  </si>
-  <si>
-    <t>66863</t>
-  </si>
-  <si>
-    <t>Automation V2 Project4672162</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>5430 Ebert Terrace</t>
-  </si>
-  <si>
-    <t>Rathport</t>
-  </si>
-  <si>
-    <t>68598</t>
-  </si>
-  <si>
-    <t>30612</t>
-  </si>
-  <si>
-    <t>2202272600</t>
-  </si>
-  <si>
-    <t>Automation V2 Project2103211</t>
-  </si>
-  <si>
-    <t>Hunan</t>
-  </si>
-  <si>
-    <t>78711 Jacqualine Garden</t>
-  </si>
-  <si>
-    <t>Pollichshire</t>
-  </si>
-  <si>
-    <t>32773-5921</t>
-  </si>
-  <si>
-    <t>45560</t>
-  </si>
-  <si>
     <t>2202272601</t>
   </si>
   <si>
-    <t>Automation V2 Project1055886</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>906 Alberto Mission</t>
-  </si>
-  <si>
-    <t>Buckridgebury</t>
-  </si>
-  <si>
-    <t>17318-3959</t>
-  </si>
-  <si>
-    <t>54864</t>
-  </si>
-  <si>
-    <t>2202272602</t>
-  </si>
-  <si>
     <t>Automation V2 Project2182532</t>
   </si>
   <si>
@@ -1136,60 +581,6 @@
     <t>18793</t>
   </si>
   <si>
-    <t>Automation V2 Project442406</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>72656 Cummings Fall</t>
-  </si>
-  <si>
-    <t>East Tyrell</t>
-  </si>
-  <si>
-    <t>07210</t>
-  </si>
-  <si>
-    <t>8532</t>
-  </si>
-  <si>
-    <t>Automation V2 Project4980327</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>076 Cartwright Hill</t>
-  </si>
-  <si>
-    <t>Joneston</t>
-  </si>
-  <si>
-    <t>75391</t>
-  </si>
-  <si>
-    <t>9712</t>
-  </si>
-  <si>
-    <t>Automation V2 Project3898382</t>
-  </si>
-  <si>
-    <t>5173 Elfreda Roads</t>
-  </si>
-  <si>
-    <t>North Diego</t>
-  </si>
-  <si>
-    <t>22038-8728</t>
-  </si>
-  <si>
-    <t>2438</t>
-  </si>
-  <si>
-    <t>2202272641</t>
-  </si>
-  <si>
     <t>Soon</t>
   </si>
   <si>
@@ -1229,141 +620,6 @@
     <t>13519-1518</t>
   </si>
   <si>
-    <t>Automation portfolio 3386090</t>
-  </si>
-  <si>
-    <t>46768</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>97348 Waters Hill</t>
-  </si>
-  <si>
-    <t>Jenellland</t>
-  </si>
-  <si>
-    <t>17304-1646</t>
-  </si>
-  <si>
-    <t>WELLP07133</t>
-  </si>
-  <si>
-    <t>Kenia</t>
-  </si>
-  <si>
-    <t>karri.gleichner@hotmail.com</t>
-  </si>
-  <si>
-    <t>0206552567</t>
-  </si>
-  <si>
-    <t>Tynisha</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2538556</t>
-  </si>
-  <si>
-    <t>Food &amp; Beverage</t>
-  </si>
-  <si>
-    <t>40313</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>400 Garry Course</t>
-  </si>
-  <si>
-    <t>Mohrtown</t>
-  </si>
-  <si>
-    <t>61642-3111</t>
-  </si>
-  <si>
-    <t>WELLP07134</t>
-  </si>
-  <si>
-    <t>Vern</t>
-  </si>
-  <si>
-    <t>felisa.crist@hotmail.com</t>
-  </si>
-  <si>
-    <t>2808075671</t>
-  </si>
-  <si>
-    <t>Giuseppe</t>
-  </si>
-  <si>
-    <t>Automation portfolio 2343247</t>
-  </si>
-  <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>35226</t>
-  </si>
-  <si>
-    <t>82753 Sandy Prairie</t>
-  </si>
-  <si>
-    <t>Lake Santos</t>
-  </si>
-  <si>
-    <t>60876</t>
-  </si>
-  <si>
-    <t>WELLP07136</t>
-  </si>
-  <si>
-    <t>Herb</t>
-  </si>
-  <si>
-    <t>rosalyn.gaylord@gmail.com</t>
-  </si>
-  <si>
-    <t>8971038170</t>
-  </si>
-  <si>
-    <t>Cruz</t>
-  </si>
-  <si>
-    <t>Automation portfolio 1695885</t>
-  </si>
-  <si>
-    <t>36706</t>
-  </si>
-  <si>
-    <t>Virgin Islands</t>
-  </si>
-  <si>
-    <t>02266 Darci Ramp</t>
-  </si>
-  <si>
-    <t>Shermanland</t>
-  </si>
-  <si>
-    <t>38555-1839</t>
-  </si>
-  <si>
-    <t>WELLP07137</t>
-  </si>
-  <si>
-    <t>Vance</t>
-  </si>
-  <si>
-    <t>millard.huels@hotmail.com</t>
-  </si>
-  <si>
-    <t>4411720046</t>
-  </si>
-  <si>
-    <t>Ulysses</t>
-  </si>
-  <si>
     <t>Automation V2 Project1904145</t>
   </si>
   <si>
@@ -1436,72 +692,6 @@
     <t>HSRP007142</t>
   </si>
   <si>
-    <t>Automation portfolio 6774762</t>
-  </si>
-  <si>
-    <t>Hospitals</t>
-  </si>
-  <si>
-    <t>12620</t>
-  </si>
-  <si>
-    <t>969 Deidre Expressway</t>
-  </si>
-  <si>
-    <t>North Jeffersonview</t>
-  </si>
-  <si>
-    <t>26745-8382</t>
-  </si>
-  <si>
-    <t>WELLP07144</t>
-  </si>
-  <si>
-    <t>Automation portfolio 4164397</t>
-  </si>
-  <si>
-    <t>Hotel</t>
-  </si>
-  <si>
-    <t>19850</t>
-  </si>
-  <si>
-    <t>36872 Legros Mews</t>
-  </si>
-  <si>
-    <t>Stephaneport</t>
-  </si>
-  <si>
-    <t>62905</t>
-  </si>
-  <si>
-    <t>WELLP07145</t>
-  </si>
-  <si>
-    <t>Viki</t>
-  </si>
-  <si>
-    <t>pamelia.cremin@gmail.com</t>
-  </si>
-  <si>
-    <t>0548554450</t>
-  </si>
-  <si>
-    <t>Dionne</t>
-  </si>
-  <si>
-    <t>Automation portfolio 3977561</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>7548</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
     <t>8456 Lind Tunnel</t>
   </si>
   <si>
@@ -1511,9 +701,6 @@
     <t>68409-2257</t>
   </si>
   <si>
-    <t>WELLP07149</t>
-  </si>
-  <si>
     <t>Traci</t>
   </si>
   <si>
@@ -1560,6 +747,72 @@
   </si>
   <si>
     <t>Alona</t>
+  </si>
+  <si>
+    <t>WELLP07185</t>
+  </si>
+  <si>
+    <t>Christy</t>
+  </si>
+  <si>
+    <t>Bambi</t>
+  </si>
+  <si>
+    <t>dakota.lubowitz@gmail.com</t>
+  </si>
+  <si>
+    <t>0114775186</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>508 Corkery Extension</t>
+  </si>
+  <si>
+    <t>Lake Olastad</t>
+  </si>
+  <si>
+    <t>Grisel</t>
+  </si>
+  <si>
+    <t>monika.bechtelar@hotmail.com</t>
+  </si>
+  <si>
+    <t>0013100742</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>8625 Hilll Mount</t>
+  </si>
+  <si>
+    <t>Waelchihaven</t>
+  </si>
+  <si>
+    <t>Melinda</t>
+  </si>
+  <si>
+    <t>Miquel</t>
+  </si>
+  <si>
+    <t>Jasper</t>
+  </si>
+  <si>
+    <t>sonny.willms@yahoo.com</t>
+  </si>
+  <si>
+    <t>7758427180</t>
+  </si>
+  <si>
+    <t>7374 Olson Ferry</t>
+  </si>
+  <si>
+    <t>West Eusebiafurt</t>
+  </si>
+  <si>
+    <t>Holly</t>
   </si>
 </sst>
 </file>
@@ -1948,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1981,27 +1234,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.23828125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.25" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.921875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="31.953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="29.62890625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.6796875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.23046875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.71875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.90234375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.62109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.12109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
@@ -2019,11 +1271,11 @@
     <col min="36" max="36" customWidth="true" width="14.5703125" collapsed="true"/>
     <col min="37" max="37" customWidth="true" width="21.140625" collapsed="true"/>
     <col min="38" max="38" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="30.609375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="9.40625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.9140625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
     <col min="42" max="42" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="8.765625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
     <col min="44" max="44" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
     <col min="45" max="45" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
     <col min="46" max="46" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
@@ -2031,7 +1283,7 @@
   <sheetData>
     <row r="1" spans="1:47">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
@@ -2061,7 +1313,7 @@
         <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L1" t="s">
         <v>17</v>
@@ -2073,19 +1325,19 @@
         <v>8</v>
       </c>
       <c r="O1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" t="s">
         <v>68</v>
       </c>
-      <c r="P1" t="s">
-        <v>69</v>
-      </c>
       <c r="Q1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" t="s">
+        <v>114</v>
+      </c>
+      <c r="S1" t="s">
         <v>116</v>
-      </c>
-      <c r="R1" t="s">
-        <v>115</v>
-      </c>
-      <c r="S1" t="s">
-        <v>117</v>
       </c>
       <c r="T1" t="s">
         <v>25</v>
@@ -2094,144 +1346,144 @@
         <v>19</v>
       </c>
       <c r="V1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" t="s">
         <v>73</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" t="s">
         <v>75</v>
       </c>
-      <c r="X1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>76</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>77</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>78</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>79</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>80</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>81</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>82</v>
       </c>
-      <c r="AL1" t="s">
-        <v>83</v>
-      </c>
       <c r="AM1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR1" t="s">
         <v>107</v>
       </c>
-      <c r="AN1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>108</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>109</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:47">
       <c r="A2" s="4" t="s">
-        <v>449</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>443</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>387</v>
+        <v>184</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>444</v>
+        <v>196</v>
       </c>
       <c r="F2" t="s">
-        <v>445</v>
+        <v>197</v>
       </c>
       <c r="G2" t="s">
-        <v>446</v>
+        <v>198</v>
       </c>
       <c r="H2" t="s">
-        <v>447</v>
+        <v>199</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>448</v>
+        <v>200</v>
       </c>
       <c r="K2" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
       <c r="L2" t="s">
-        <v>385</v>
+        <v>182</v>
       </c>
       <c r="M2" t="s">
-        <v>386</v>
+        <v>183</v>
       </c>
       <c r="N2" t="s">
-        <v>388</v>
+        <v>185</v>
       </c>
       <c r="O2" t="s">
         <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>389</v>
+        <v>186</v>
       </c>
       <c r="Q2" t="s">
-        <v>390</v>
+        <v>187</v>
       </c>
       <c r="R2" t="s">
-        <v>391</v>
+        <v>188</v>
       </c>
       <c r="S2" t="s">
-        <v>392</v>
+        <v>189</v>
       </c>
       <c r="T2" t="s">
-        <v>385</v>
+        <v>182</v>
       </c>
       <c r="U2" t="s">
-        <v>393</v>
+        <v>190</v>
       </c>
       <c r="V2" t="s">
         <v>31</v>
@@ -2243,136 +1495,136 @@
         <v>33</v>
       </c>
       <c r="Y2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="Z2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="AA2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="AB2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC2" t="s">
         <v>12</v>
       </c>
       <c r="AD2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AE2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF2" t="s">
         <v>84</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>85</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>86</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>87</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>88</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>89</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>90</v>
       </c>
-      <c r="AL2" t="s">
-        <v>91</v>
-      </c>
       <c r="AM2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AO2" s="5" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="AP2" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AU2" s="6"/>
     </row>
     <row r="3" spans="1:47">
       <c r="A3" s="5" t="s">
-        <v>353</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>361</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>362</v>
+        <v>177</v>
       </c>
       <c r="F3" t="s">
-        <v>363</v>
+        <v>178</v>
       </c>
       <c r="G3" t="s">
-        <v>364</v>
+        <v>179</v>
       </c>
       <c r="H3" t="s">
-        <v>365</v>
+        <v>180</v>
       </c>
       <c r="I3" t="s">
         <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>366</v>
+        <v>181</v>
       </c>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L3" t="s">
+        <v>117</v>
+      </c>
+      <c r="M3" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" t="s">
         <v>121</v>
       </c>
-      <c r="M3" t="s">
+      <c r="R3" t="s">
         <v>122</v>
       </c>
-      <c r="N3" t="s">
-        <v>101</v>
-      </c>
-      <c r="O3" t="s">
-        <v>112</v>
-      </c>
-      <c r="P3" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>125</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
+        <v>123</v>
+      </c>
+      <c r="T3" t="s">
+        <v>117</v>
+      </c>
+      <c r="U3" t="s">
         <v>126</v>
-      </c>
-      <c r="S3" t="s">
-        <v>127</v>
-      </c>
-      <c r="T3" t="s">
-        <v>121</v>
-      </c>
-      <c r="U3" t="s">
-        <v>130</v>
       </c>
       <c r="V3" t="s">
         <v>31</v>
@@ -2384,37 +1636,37 @@
         <v>33</v>
       </c>
       <c r="AB3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC3" t="s">
         <v>12</v>
       </c>
       <c r="AD3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AE3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF3" t="s">
         <v>84</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>85</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>86</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>87</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>88</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>89</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>90</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2428,45 +1680,44 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.62890625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.6796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="27.1171875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.80078125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.859375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.31640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.15625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="41.45703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="41.42578125" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="24" max="24" customWidth="true" width="37.5703125" collapsed="true"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="11.4609375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.40234375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="28" max="29" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -2475,16 +1726,16 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
@@ -2508,102 +1759,102 @@
         <v>18</v>
       </c>
       <c r="O1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P1" t="s">
         <v>19</v>
       </c>
       <c r="Q1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" t="s">
         <v>73</v>
       </c>
-      <c r="R1" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" t="s">
-        <v>74</v>
-      </c>
       <c r="T1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="U1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="W1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="X1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="Y1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="Z1" t="s">
         <v>13</v>
       </c>
       <c r="AA1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="AB1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="AC1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="AD1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="30">
       <c r="A2" t="s">
-        <v>492</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s">
-        <v>498</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
-        <v>499</v>
+        <v>228</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
       <c r="G2" t="s">
-        <v>500</v>
+        <v>229</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>254</v>
+        <v>172</v>
       </c>
       <c r="J2" t="s">
-        <v>489</v>
+        <v>219</v>
       </c>
       <c r="K2" t="s">
-        <v>490</v>
+        <v>220</v>
       </c>
       <c r="L2" t="s">
-        <v>491</v>
+        <v>221</v>
       </c>
       <c r="M2" t="s">
-        <v>493</v>
+        <v>222</v>
       </c>
       <c r="N2" t="s">
-        <v>494</v>
+        <v>223</v>
       </c>
       <c r="O2" t="s">
-        <v>495</v>
+        <v>224</v>
       </c>
       <c r="P2" t="s">
-        <v>496</v>
+        <v>225</v>
       </c>
       <c r="Q2" t="s">
         <v>31</v>
@@ -2615,37 +1866,37 @@
         <v>33</v>
       </c>
       <c r="T2" t="s">
-        <v>326</v>
+        <v>174</v>
       </c>
       <c r="U2" t="s">
+        <v>147</v>
+      </c>
+      <c r="V2" t="s">
+        <v>146</v>
+      </c>
+      <c r="W2" t="s">
+        <v>148</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA2" t="s">
         <v>160</v>
       </c>
-      <c r="V2" t="s">
-        <v>159</v>
-      </c>
-      <c r="W2" t="s">
-        <v>161</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>174</v>
-      </c>
       <c r="AB2" t="s">
-        <v>497</v>
+        <v>226</v>
       </c>
       <c r="AC2" t="s">
-        <v>250</v>
+        <v>171</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2664,14 +1915,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.234375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.2578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.16015625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.64453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.71875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2691,39 +1942,39 @@
         <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
-        <v>46</v>
-      </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>394</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>395</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>396</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
-        <v>397</v>
+        <v>194</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -2767,7 +2018,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
@@ -2785,72 +2036,72 @@
         <v>22</v>
       </c>
       <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>41</v>
-      </c>
-      <c r="L1" t="s">
-        <v>42</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" t="s">
         <v>73</v>
-      </c>
-      <c r="O1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
         <v>92</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>93</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
-        <v>95</v>
-      </c>
       <c r="H2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
         <v>97</v>
       </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
         <v>98</v>
-      </c>
-      <c r="K2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" t="s">
-        <v>99</v>
       </c>
       <c r="N2" t="s">
         <v>31</v>
@@ -2878,18 +2129,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="30.95703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.6953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="23.53515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.60546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.94921875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="31.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
@@ -2902,13 +2153,13 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -2929,7 +2180,7 @@
         <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s">
         <v>15</v>
@@ -2938,78 +2189,78 @@
         <v>19</v>
       </c>
       <c r="M1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" t="s">
-        <v>77</v>
-      </c>
       <c r="R1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S1" t="s">
+        <v>151</v>
+      </c>
+      <c r="T1" t="s">
         <v>152</v>
       </c>
-      <c r="S1" t="s">
-        <v>165</v>
-      </c>
-      <c r="T1" t="s">
-        <v>166</v>
-      </c>
       <c r="U1" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="V1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="W1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="X1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
-        <v>466</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>458</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>459</v>
+        <v>211</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>460</v>
+        <v>212</v>
       </c>
       <c r="G2" t="s">
-        <v>461</v>
+        <v>213</v>
       </c>
       <c r="H2" t="s">
-        <v>462</v>
+        <v>214</v>
       </c>
       <c r="I2" t="s">
-        <v>463</v>
+        <v>215</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>464</v>
+        <v>216</v>
       </c>
       <c r="L2" t="s">
-        <v>465</v>
+        <v>217</v>
       </c>
       <c r="M2" t="s">
         <v>31</v>
@@ -3021,31 +2272,31 @@
         <v>33</v>
       </c>
       <c r="P2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S2" t="s">
+        <v>154</v>
+      </c>
+      <c r="T2" t="s">
+        <v>155</v>
+      </c>
+      <c r="U2" t="s">
+        <v>162</v>
+      </c>
+      <c r="V2" t="s">
+        <v>164</v>
+      </c>
+      <c r="W2" t="s">
         <v>163</v>
       </c>
-      <c r="Q2" t="s">
-        <v>164</v>
-      </c>
-      <c r="R2" t="s">
-        <v>167</v>
-      </c>
-      <c r="S2" t="s">
-        <v>168</v>
-      </c>
-      <c r="T2" t="s">
-        <v>169</v>
-      </c>
-      <c r="U2" t="s">
-        <v>176</v>
-      </c>
-      <c r="V2" t="s">
-        <v>178</v>
-      </c>
-      <c r="W2" t="s">
-        <v>177</v>
-      </c>
       <c r="X2" s="5" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3063,19 +2314,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.015625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.171875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.8203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.76953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.29296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.23046875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.171875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.44921875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.39453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.86328125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
@@ -3088,7 +2339,7 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -3100,7 +2351,7 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -3127,84 +2378,84 @@
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>75</v>
       </c>
-      <c r="P1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" t="s">
-        <v>77</v>
-      </c>
       <c r="S1" t="s">
+        <v>139</v>
+      </c>
+      <c r="T1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U1" t="s">
         <v>152</v>
       </c>
-      <c r="T1" t="s">
-        <v>165</v>
-      </c>
-      <c r="U1" t="s">
-        <v>166</v>
-      </c>
       <c r="V1" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="W1" t="s">
         <v>15</v>
       </c>
       <c r="X1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="Y1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="Z1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>457</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>451</v>
+        <v>203</v>
       </c>
       <c r="G2" t="s">
-        <v>452</v>
+        <v>204</v>
       </c>
       <c r="H2" t="s">
-        <v>453</v>
+        <v>205</v>
       </c>
       <c r="I2" t="s">
-        <v>454</v>
+        <v>206</v>
       </c>
       <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
       <c r="L2" t="s">
-        <v>455</v>
+        <v>207</v>
       </c>
       <c r="M2" t="s">
-        <v>456</v>
+        <v>208</v>
       </c>
       <c r="N2" t="s">
         <v>31</v>
@@ -3216,28 +2467,28 @@
         <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="R2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="S2" t="s">
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="T2" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="U2" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="V2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="W2">
         <v>48698</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3261,7 +2512,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3280,15 +2531,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="33.01953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.37109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.5234375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="7.96875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.78515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.62109375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="12.4921875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.36328125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.07421875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.6953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.671875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.69140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.97265625" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
@@ -3297,16 +2548,16 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>14</v>
@@ -3315,10 +2566,10 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
         <v>21</v>
@@ -3330,48 +2581,48 @@
         <v>19</v>
       </c>
       <c r="L1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" t="s">
         <v>73</v>
-      </c>
-      <c r="M1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>503</v>
+        <v>255</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>504</v>
+        <v>256</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>505</v>
+        <v>249</v>
       </c>
       <c r="G2" t="s">
-        <v>501</v>
+        <v>253</v>
       </c>
       <c r="H2" t="s">
-        <v>502</v>
+        <v>254</v>
       </c>
       <c r="I2" t="s">
-        <v>507</v>
+        <v>258</v>
       </c>
       <c r="J2" t="s">
-        <v>506</v>
+        <v>257</v>
       </c>
       <c r="K2" t="s">
-        <v>508</v>
+        <v>259</v>
       </c>
       <c r="L2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
changed user email id
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7572CB26-1044-418C-A4AF-00C6304E06DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A740F0-38A8-4A8F-94BC-1A20631AE70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="260">
   <si>
     <t>UserName</t>
   </si>
@@ -305,33 +305,6 @@
     <t>BillingNote Test</t>
   </si>
   <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>08201 Rohan Glen</t>
-  </si>
-  <si>
-    <t>Wymanbury</t>
-  </si>
-  <si>
-    <t>48650</t>
-  </si>
-  <si>
-    <t>3332769997</t>
-  </si>
-  <si>
-    <t>Abe</t>
-  </si>
-  <si>
-    <t>Management Consulting</t>
-  </si>
-  <si>
-    <t>Nicol</t>
-  </si>
-  <si>
-    <t>w633e80d90291d</t>
-  </si>
-  <si>
     <t>Oil &amp; Gas</t>
   </si>
   <si>
@@ -488,15 +461,6 @@
     <t>WellReviewer</t>
   </si>
   <si>
-    <t>Shekhar (shekhar.chikara@wellcertified.com)</t>
-  </si>
-  <si>
-    <t>Eleftherios (eleftherios.zacharakis@wellcertified.com)</t>
-  </si>
-  <si>
-    <t>Marc (Marc@gbci.org)</t>
-  </si>
-  <si>
     <t>ProjectVersion</t>
   </si>
   <si>
@@ -548,638 +512,313 @@
     <t>Karen (karen.quintana@wellcertified.com)</t>
   </si>
   <si>
-    <t>2202272601</t>
-  </si>
-  <si>
-    <t>Automation V2 Project2182532</t>
-  </si>
-  <si>
-    <t>Qinghai</t>
-  </si>
-  <si>
-    <t>810 Effertz Locks</t>
-  </si>
-  <si>
-    <t>South Cameronfort</t>
-  </si>
-  <si>
-    <t>40046-1711</t>
-  </si>
-  <si>
-    <t>18793</t>
-  </si>
-  <si>
-    <t>Soon</t>
-  </si>
-  <si>
-    <t>emmett.dietrich@hotmail.com</t>
-  </si>
-  <si>
-    <t>5580505887</t>
-  </si>
-  <si>
-    <t>Personal Finance</t>
+    <t>Retail Spaces</t>
+  </si>
+  <si>
+    <t>welluiautomationtesting@gmail.com</t>
+  </si>
+  <si>
+    <t>WELLP07239</t>
+  </si>
+  <si>
+    <t>Allyson</t>
+  </si>
+  <si>
+    <t>kristle.gleason@hotmail.com</t>
+  </si>
+  <si>
+    <t>4083649132</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>WERSelectMember</t>
+  </si>
+  <si>
+    <t>WERlocations</t>
+  </si>
+  <si>
+    <t>WERlocationsize</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>Ui (welluiautomationtesting@gmail.com)</t>
+  </si>
+  <si>
+    <t>Cristobal</t>
+  </si>
+  <si>
+    <t>roderick.corwin@gmail.com</t>
+  </si>
+  <si>
+    <t>6178045462</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>520 Runte Alley</t>
+  </si>
+  <si>
+    <t>West Manside</t>
+  </si>
+  <si>
+    <t>86735</t>
+  </si>
+  <si>
+    <t>Gavin</t>
+  </si>
+  <si>
+    <t>Automation V2 Project4937302</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>567 Kulas Islands</t>
+  </si>
+  <si>
+    <t>Reubenfurt</t>
+  </si>
+  <si>
+    <t>17686-5899</t>
+  </si>
+  <si>
+    <t>25974</t>
+  </si>
+  <si>
+    <t>2202274588</t>
+  </si>
+  <si>
+    <t>Automation V2 Project6287139</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>6849 Brown Pass</t>
+  </si>
+  <si>
+    <t>South Sundaymouth</t>
+  </si>
+  <si>
+    <t>27877-4018</t>
+  </si>
+  <si>
+    <t>84458</t>
+  </si>
+  <si>
+    <t>2202274589</t>
+  </si>
+  <si>
+    <t>Automation HSR Project 962241</t>
+  </si>
+  <si>
+    <t>Theater</t>
+  </si>
+  <si>
+    <t>57800 Cammie Stream</t>
+  </si>
+  <si>
+    <t>West Jesse</t>
+  </si>
+  <si>
+    <t>60135-0924</t>
+  </si>
+  <si>
+    <t>23093</t>
+  </si>
+  <si>
+    <t>Kaila</t>
+  </si>
+  <si>
+    <t>HSRP007371</t>
+  </si>
+  <si>
+    <t>Automation WPR Project4176554</t>
+  </si>
+  <si>
+    <t>Affordable Housing</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>558 Penney Centers</t>
+  </si>
+  <si>
+    <t>Purdyburgh</t>
+  </si>
+  <si>
+    <t>14028-2622</t>
+  </si>
+  <si>
+    <t>41926</t>
+  </si>
+  <si>
+    <t>Romeo</t>
+  </si>
+  <si>
+    <t>WPR007372</t>
+  </si>
+  <si>
+    <t>Automation portfolio 7183304</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>5960</t>
+  </si>
+  <si>
+    <t>6898 Purdy Fort</t>
+  </si>
+  <si>
+    <t>Fayberg</t>
+  </si>
+  <si>
+    <t>06787-2048</t>
+  </si>
+  <si>
+    <t>0135 Becker Mall</t>
+  </si>
+  <si>
+    <t>East Cruzfort</t>
+  </si>
+  <si>
+    <t>69858</t>
+  </si>
+  <si>
+    <t>6868036304</t>
+  </si>
+  <si>
+    <t>Octavio</t>
+  </si>
+  <si>
+    <t>Online Media</t>
+  </si>
+  <si>
+    <t>Adele</t>
+  </si>
+  <si>
+    <t>w63761f89519da</t>
+  </si>
+  <si>
+    <t>Automation WER Project7138568</t>
+  </si>
+  <si>
+    <t>Corporate Real Estate</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>308 Deckow Mountain</t>
+  </si>
+  <si>
+    <t>North Judeville</t>
+  </si>
+  <si>
+    <t>22816-3365</t>
+  </si>
+  <si>
+    <t>15481</t>
+  </si>
+  <si>
+    <t>Elina</t>
+  </si>
+  <si>
+    <t>Classroom</t>
+  </si>
+  <si>
+    <t>WER007458</t>
+  </si>
+  <si>
+    <t>Alvin</t>
+  </si>
+  <si>
+    <t>Ricky</t>
+  </si>
+  <si>
+    <t>edgar.schiller@hotmail.com</t>
+  </si>
+  <si>
+    <t>6793518182</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>437 DuBuque Crossroad</t>
+  </si>
+  <si>
+    <t>Runolfsdottirfort</t>
+  </si>
+  <si>
+    <t>Eugenie</t>
   </si>
   <si>
     <t>Iowa</t>
   </si>
   <si>
-    <t>6146 Marian Corners</t>
-  </si>
-  <si>
-    <t>West Cindafort</t>
-  </si>
-  <si>
-    <t>42470-6776</t>
-  </si>
-  <si>
-    <t>Refugio</t>
-  </si>
-  <si>
-    <t>Automation V2 Project1904145</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>1881 O'Reilly Underpass</t>
-  </si>
-  <si>
-    <t>East Robert</t>
-  </si>
-  <si>
-    <t>78878-5342</t>
-  </si>
-  <si>
-    <t>66082</t>
-  </si>
-  <si>
-    <t>2202272937</t>
-  </si>
-  <si>
-    <t>Automation WPR Project2128589</t>
-  </si>
-  <si>
-    <t>Packing &amp; Shipping</t>
-  </si>
-  <si>
-    <t>8120 Wilderman Trail</t>
-  </si>
-  <si>
-    <t>South Mohamedport</t>
-  </si>
-  <si>
-    <t>84305</t>
-  </si>
-  <si>
-    <t>47364</t>
-  </si>
-  <si>
-    <t>Liliana</t>
-  </si>
-  <si>
-    <t>WPR007141</t>
-  </si>
-  <si>
-    <t>Automation HSR Project 1138515</t>
-  </si>
-  <si>
-    <t>Travel Support</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>24591 Murphy Hills</t>
-  </si>
-  <si>
-    <t>East Thedaview</t>
-  </si>
-  <si>
-    <t>37929</t>
-  </si>
-  <si>
-    <t>11400</t>
-  </si>
-  <si>
-    <t>Sammy</t>
-  </si>
-  <si>
-    <t>HSRP007142</t>
-  </si>
-  <si>
-    <t>Retail Spaces</t>
-  </si>
-  <si>
-    <t>Xenia</t>
-  </si>
-  <si>
-    <t>Myrle</t>
-  </si>
-  <si>
-    <t>lewis.thiel@hotmail.com</t>
-  </si>
-  <si>
-    <t>2687605502</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>219 Borer Grove</t>
-  </si>
-  <si>
-    <t>East Danille</t>
-  </si>
-  <si>
-    <t>Alona</t>
-  </si>
-  <si>
-    <t>welluiautomationtesting@gmail.com</t>
-  </si>
-  <si>
-    <t>abhishek.gupta@wellcertified.com</t>
-  </si>
-  <si>
-    <t>Virgin Islands</t>
-  </si>
-  <si>
-    <t>308 Larry Springs</t>
-  </si>
-  <si>
-    <t>Borershire</t>
-  </si>
-  <si>
-    <t>19428-1862</t>
-  </si>
-  <si>
-    <t>Automation portfolio 938140</t>
-  </si>
-  <si>
-    <t>Investment Services</t>
-  </si>
-  <si>
-    <t>25161</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>385 Royce Light</t>
-  </si>
-  <si>
-    <t>Reynaldaville</t>
-  </si>
-  <si>
-    <t>09857</t>
-  </si>
-  <si>
-    <t>WELLP07239</t>
-  </si>
-  <si>
-    <t>Allyson</t>
-  </si>
-  <si>
-    <t>kristle.gleason@hotmail.com</t>
-  </si>
-  <si>
-    <t>4083649132</t>
-  </si>
-  <si>
-    <t>Miss</t>
-  </si>
-  <si>
-    <t>WERSelectMember</t>
-  </si>
-  <si>
-    <t>WERlocations</t>
-  </si>
-  <si>
-    <t>WERlocationsize</t>
-  </si>
-  <si>
-    <t>Automation WER Project4296902</t>
-  </si>
-  <si>
-    <t>Post Secondary Education</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>079 Skiles Springs</t>
-  </si>
-  <si>
-    <t>New Chanelle</t>
-  </si>
-  <si>
-    <t>33687</t>
-  </si>
-  <si>
-    <t>19486</t>
-  </si>
-  <si>
-    <t>Adelle</t>
-  </si>
-  <si>
-    <t>WER007280</t>
-  </si>
-  <si>
-    <t>Ui (welluiautomationtesting@gmail.com)</t>
-  </si>
-  <si>
-    <t>Guam</t>
-  </si>
-  <si>
-    <t>9183 Metz Trail</t>
-  </si>
-  <si>
-    <t>East Phebe</t>
-  </si>
-  <si>
-    <t>78761-5594</t>
-  </si>
-  <si>
-    <t>5347548011</t>
-  </si>
-  <si>
-    <t>Janella</t>
-  </si>
-  <si>
-    <t>101 Moorgate</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>1617 Kuphal Isle</t>
-  </si>
-  <si>
-    <t>East Kingside</t>
-  </si>
-  <si>
-    <t>90732-2581</t>
-  </si>
-  <si>
-    <t>1876690099</t>
-  </si>
-  <si>
-    <t>Lucia</t>
-  </si>
-  <si>
-    <t>Real estate</t>
-  </si>
-  <si>
-    <t>American Samoa</t>
-  </si>
-  <si>
-    <t>92118 Lino Manor</t>
-  </si>
-  <si>
-    <t>Robenafort</t>
-  </si>
-  <si>
-    <t>85773</t>
-  </si>
-  <si>
-    <t>7552433047</t>
-  </si>
-  <si>
-    <t>Delana</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>3029 Lenora View</t>
-  </si>
-  <si>
-    <t>New Peggie</t>
-  </si>
-  <si>
-    <t>04767</t>
-  </si>
-  <si>
-    <t>5687743163</t>
-  </si>
-  <si>
-    <t>Bruce</t>
-  </si>
-  <si>
-    <t>Health, Wellness &amp; Fitness</t>
-  </si>
-  <si>
-    <t>Automation V2 Project5253236</t>
-  </si>
-  <si>
-    <t>71796 O'Connell Island</t>
-  </si>
-  <si>
-    <t>Port Brendonbury</t>
-  </si>
-  <si>
-    <t>30992-0572</t>
-  </si>
-  <si>
-    <t>Automation WPR Project272898</t>
-  </si>
-  <si>
-    <t>Wellness Services</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>964 Ziemann Prairie</t>
-  </si>
-  <si>
-    <t>Lake Rafaeltown</t>
-  </si>
-  <si>
-    <t>76506-9821</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>962 Hayden Mall</t>
-  </si>
-  <si>
-    <t>Keshaville</t>
-  </si>
-  <si>
-    <t>46711-8912</t>
-  </si>
-  <si>
-    <t>1157864623</t>
-  </si>
-  <si>
-    <t>Otto</t>
-  </si>
-  <si>
-    <t>Legal</t>
-  </si>
-  <si>
-    <t>Shelton</t>
-  </si>
-  <si>
-    <t>w6376044de063c</t>
-  </si>
-  <si>
-    <t>1789 Beier Ferry</t>
-  </si>
-  <si>
-    <t>East Abe</t>
-  </si>
-  <si>
-    <t>29433</t>
-  </si>
-  <si>
-    <t>Automation V2 Project5630100</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>8637 Mraz Circle</t>
-  </si>
-  <si>
-    <t>Mayertborough</t>
-  </si>
-  <si>
-    <t>86981</t>
-  </si>
-  <si>
-    <t>843</t>
-  </si>
-  <si>
-    <t>2202274587</t>
-  </si>
-  <si>
-    <t>Cristobal</t>
-  </si>
-  <si>
-    <t>roderick.corwin@gmail.com</t>
-  </si>
-  <si>
-    <t>6178045462</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>520 Runte Alley</t>
-  </si>
-  <si>
-    <t>West Manside</t>
-  </si>
-  <si>
-    <t>86735</t>
-  </si>
-  <si>
-    <t>Gavin</t>
-  </si>
-  <si>
-    <t>Automation V2 Project4937302</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>567 Kulas Islands</t>
-  </si>
-  <si>
-    <t>Reubenfurt</t>
-  </si>
-  <si>
-    <t>17686-5899</t>
-  </si>
-  <si>
-    <t>25974</t>
-  </si>
-  <si>
-    <t>2202274588</t>
-  </si>
-  <si>
-    <t>Automation V2 Project6287139</t>
-  </si>
-  <si>
-    <t>Beijing</t>
-  </si>
-  <si>
-    <t>6849 Brown Pass</t>
-  </si>
-  <si>
-    <t>South Sundaymouth</t>
-  </si>
-  <si>
-    <t>27877-4018</t>
-  </si>
-  <si>
-    <t>84458</t>
-  </si>
-  <si>
-    <t>2202274589</t>
-  </si>
-  <si>
-    <t>Automation HSR Project 962241</t>
-  </si>
-  <si>
-    <t>Theater</t>
-  </si>
-  <si>
-    <t>57800 Cammie Stream</t>
-  </si>
-  <si>
-    <t>West Jesse</t>
-  </si>
-  <si>
-    <t>60135-0924</t>
-  </si>
-  <si>
-    <t>23093</t>
-  </si>
-  <si>
-    <t>Kaila</t>
-  </si>
-  <si>
-    <t>HSRP007371</t>
-  </si>
-  <si>
-    <t>Automation WPR Project4176554</t>
-  </si>
-  <si>
-    <t>Affordable Housing</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>558 Penney Centers</t>
-  </si>
-  <si>
-    <t>Purdyburgh</t>
-  </si>
-  <si>
-    <t>14028-2622</t>
-  </si>
-  <si>
-    <t>41926</t>
-  </si>
-  <si>
-    <t>Romeo</t>
-  </si>
-  <si>
-    <t>WPR007372</t>
-  </si>
-  <si>
-    <t>Automation portfolio 7183304</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>5960</t>
-  </si>
-  <si>
-    <t>6898 Purdy Fort</t>
-  </si>
-  <si>
-    <t>Fayberg</t>
-  </si>
-  <si>
-    <t>06787-2048</t>
-  </si>
-  <si>
-    <t>Automation portfolio 5790377</t>
-  </si>
-  <si>
-    <t>Primary or Secondary Education</t>
-  </si>
-  <si>
-    <t>1858</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>69590 Spinka Stravenue</t>
-  </si>
-  <si>
-    <t>Hueyville</t>
-  </si>
-  <si>
-    <t>67567</t>
-  </si>
-  <si>
-    <t>WELLP07374</t>
-  </si>
-  <si>
-    <t>Raymond</t>
-  </si>
-  <si>
-    <t>reva.sanford@hotmail.com</t>
-  </si>
-  <si>
-    <t>5285886243</t>
-  </si>
-  <si>
-    <t>Hung</t>
-  </si>
-  <si>
-    <t>Loise</t>
-  </si>
-  <si>
-    <t>0135 Becker Mall</t>
-  </si>
-  <si>
-    <t>East Cruzfort</t>
-  </si>
-  <si>
-    <t>69858</t>
-  </si>
-  <si>
-    <t>6868036304</t>
-  </si>
-  <si>
-    <t>Octavio</t>
-  </si>
-  <si>
-    <t>Online Media</t>
-  </si>
-  <si>
-    <t>Adele</t>
-  </si>
-  <si>
-    <t>w63761f89519da</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>0476 McLaughlin Spur</t>
-  </si>
-  <si>
-    <t>North Kelli</t>
-  </si>
-  <si>
-    <t>14680-2303</t>
+    <t>54479 Schumm View</t>
+  </si>
+  <si>
+    <t>Port Harleyport</t>
+  </si>
+  <si>
+    <t>48147-6474</t>
+  </si>
+  <si>
+    <t>Katheleen</t>
+  </si>
+  <si>
+    <t>Automation portfolio 4264460</t>
+  </si>
+  <si>
+    <t>NGOs, Non-profit Charitable Organizations</t>
+  </si>
+  <si>
+    <t>24668</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>7043 Darren Drive</t>
+  </si>
+  <si>
+    <t>New Harrisstad</t>
+  </si>
+  <si>
+    <t>94236</t>
+  </si>
+  <si>
+    <t>WELLP07472</t>
+  </si>
+  <si>
+    <t>Lane</t>
+  </si>
+  <si>
+    <t>lorenza.weimann@hotmail.com</t>
+  </si>
+  <si>
+    <t>4322747982</t>
+  </si>
+  <si>
+    <t>Dionne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1535,14 +1174,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1572,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>221</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1605,52 +1244,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.9296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.2421875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.25" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.921875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="31.953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="28.86328125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.17578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.23046875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.71875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="14.5625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.12109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="30.609375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="9.40625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.9140625" collapsed="true"/>
-    <col min="42" max="42" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="8.765625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="22" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="21" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="15" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47">
@@ -1703,13 +1342,13 @@
         <v>68</v>
       </c>
       <c r="Q1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="R1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="S1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="T1" t="s">
         <v>25</v>
@@ -1727,13 +1366,13 @@
         <v>72</v>
       </c>
       <c r="Y1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="Z1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AA1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="AB1" t="s">
         <v>61</v>
@@ -1769,93 +1408,93 @@
         <v>81</v>
       </c>
       <c r="AM1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="AN1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AO1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="AP1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AQ1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="AR1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AS1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="AT1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:47">
       <c r="A2" s="4" t="s">
-        <v>324</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>311</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>319</v>
+        <v>181</v>
       </c>
       <c r="F2" t="s">
-        <v>320</v>
+        <v>182</v>
       </c>
       <c r="G2" t="s">
-        <v>321</v>
+        <v>183</v>
       </c>
       <c r="H2" t="s">
-        <v>322</v>
+        <v>184</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>323</v>
+        <v>185</v>
       </c>
       <c r="K2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="L2" t="s">
-        <v>309</v>
+        <v>171</v>
       </c>
       <c r="M2" t="s">
-        <v>310</v>
+        <v>172</v>
       </c>
       <c r="N2" t="s">
-        <v>312</v>
+        <v>174</v>
       </c>
       <c r="O2" t="s">
         <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>313</v>
+        <v>175</v>
       </c>
       <c r="Q2" t="s">
-        <v>314</v>
+        <v>176</v>
       </c>
       <c r="R2" t="s">
-        <v>315</v>
+        <v>177</v>
       </c>
       <c r="S2" t="s">
-        <v>316</v>
+        <v>178</v>
       </c>
       <c r="T2" t="s">
-        <v>309</v>
+        <v>171</v>
       </c>
       <c r="U2" t="s">
-        <v>317</v>
+        <v>179</v>
       </c>
       <c r="V2" t="s">
         <v>31</v>
@@ -1867,13 +1506,13 @@
         <v>33</v>
       </c>
       <c r="Y2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="Z2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="AA2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="AB2" t="s">
         <v>63</v>
@@ -1882,7 +1521,7 @@
         <v>12</v>
       </c>
       <c r="AD2" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
       <c r="AE2" t="s">
         <v>82</v>
@@ -1909,94 +1548,94 @@
         <v>89</v>
       </c>
       <c r="AM2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AO2" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="AP2" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="AU2" s="6"/>
     </row>
     <row r="3" spans="1:47">
       <c r="A3" s="5" t="s">
-        <v>331</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>326</v>
+        <v>188</v>
       </c>
       <c r="F3" t="s">
-        <v>327</v>
+        <v>189</v>
       </c>
       <c r="G3" t="s">
-        <v>328</v>
+        <v>190</v>
       </c>
       <c r="H3" t="s">
-        <v>329</v>
+        <v>191</v>
       </c>
       <c r="I3" t="s">
         <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>330</v>
+        <v>192</v>
       </c>
       <c r="K3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="L3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R3" t="s">
+        <v>112</v>
+      </c>
+      <c r="S3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T3" t="s">
+        <v>107</v>
+      </c>
+      <c r="U3" t="s">
         <v>116</v>
-      </c>
-      <c r="M3" t="s">
-        <v>117</v>
-      </c>
-      <c r="N3" t="s">
-        <v>99</v>
-      </c>
-      <c r="O3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P3" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>120</v>
-      </c>
-      <c r="R3" t="s">
-        <v>121</v>
-      </c>
-      <c r="S3" t="s">
-        <v>122</v>
-      </c>
-      <c r="T3" t="s">
-        <v>116</v>
-      </c>
-      <c r="U3" t="s">
-        <v>125</v>
       </c>
       <c r="V3" t="s">
         <v>31</v>
@@ -2014,7 +1653,7 @@
         <v>12</v>
       </c>
       <c r="AD3" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
       <c r="AE3" t="s">
         <v>82</v>
@@ -2058,35 +1697,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.62890625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.93359375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.6953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="27.1171875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.80078125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.14453125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.37890625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.8515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="27.171875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="41.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="41.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -2148,37 +1787,37 @@
         <v>72</v>
       </c>
       <c r="T1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="U1" t="s">
         <v>79</v>
       </c>
       <c r="V1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="W1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="X1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="Y1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="Z1" t="s">
         <v>13</v>
       </c>
       <c r="AA1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="AB1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="AC1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="AD1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AE1" t="s">
         <v>69</v>
@@ -2186,16 +1825,16 @@
     </row>
     <row r="2" spans="1:31" ht="30">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>349</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>350</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
         <v>59</v>
@@ -2204,34 +1843,34 @@
         <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>351</v>
+        <v>213</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>243</v>
+        <v>169</v>
       </c>
       <c r="J2" t="s">
-        <v>352</v>
+        <v>214</v>
       </c>
       <c r="K2" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
       <c r="L2" t="s">
-        <v>354</v>
+        <v>216</v>
       </c>
       <c r="M2" t="s">
-        <v>234</v>
+        <v>162</v>
       </c>
       <c r="N2" t="s">
-        <v>235</v>
+        <v>163</v>
       </c>
       <c r="O2" t="s">
-        <v>236</v>
+        <v>164</v>
       </c>
       <c r="P2" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="Q2" t="s">
         <v>31</v>
@@ -2243,51 +1882,51 @@
         <v>33</v>
       </c>
       <c r="T2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="U2" t="s">
+        <v>136</v>
+      </c>
+      <c r="V2" t="s">
+        <v>135</v>
+      </c>
+      <c r="W2" t="s">
+        <v>137</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z2" t="s">
         <v>145</v>
       </c>
-      <c r="V2" t="s">
-        <v>144</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="AA2" t="s">
         <v>146</v>
       </c>
-      <c r="X2" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>158</v>
-      </c>
       <c r="AB2" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="AC2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="AE2" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="30">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
-        <v>355</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s">
-        <v>356</v>
+        <v>249</v>
       </c>
       <c r="D3" t="s">
         <v>65</v>
@@ -2299,34 +1938,34 @@
         <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>357</v>
+        <v>250</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>358</v>
+        <v>251</v>
       </c>
       <c r="J3" t="s">
-        <v>359</v>
+        <v>252</v>
       </c>
       <c r="K3" t="s">
-        <v>360</v>
+        <v>253</v>
       </c>
       <c r="L3" t="s">
-        <v>361</v>
+        <v>254</v>
       </c>
       <c r="M3" t="s">
-        <v>363</v>
+        <v>256</v>
       </c>
       <c r="N3" t="s">
-        <v>364</v>
+        <v>257</v>
       </c>
       <c r="O3" t="s">
-        <v>365</v>
+        <v>258</v>
       </c>
       <c r="P3" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="Q3" t="s">
         <v>31</v>
@@ -2338,40 +1977,40 @@
         <v>33</v>
       </c>
       <c r="T3" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="U3" t="s">
+        <v>136</v>
+      </c>
+      <c r="V3" t="s">
+        <v>135</v>
+      </c>
+      <c r="W3" t="s">
+        <v>137</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z3" t="s">
         <v>145</v>
       </c>
-      <c r="V3" t="s">
-        <v>144</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="AA3" t="s">
         <v>146</v>
       </c>
-      <c r="X3" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>158</v>
-      </c>
       <c r="AB3" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="AC3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="AD3" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="AE3" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2390,18 +2029,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.0625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.78515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.78515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.64453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.71875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2450,16 +2089,16 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>376</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
-        <v>377</v>
+        <v>244</v>
       </c>
       <c r="D2" t="s">
-        <v>378</v>
+        <v>245</v>
       </c>
       <c r="E2" t="s">
-        <v>379</v>
+        <v>246</v>
       </c>
       <c r="F2" t="s">
         <v>43</v>
@@ -2471,7 +2110,7 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>247</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
@@ -2498,22 +2137,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.48828125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.58203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.1484375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.94921875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.04296875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="19.6953125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.828125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.95703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -2568,34 +2207,34 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
-        <v>375</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>220</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>368</v>
+        <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>218</v>
       </c>
       <c r="G2" t="s">
-        <v>370</v>
+        <v>219</v>
       </c>
       <c r="H2" t="s">
-        <v>372</v>
+        <v>221</v>
       </c>
       <c r="I2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>373</v>
+        <v>222</v>
       </c>
       <c r="K2" t="s">
         <v>42</v>
@@ -2604,7 +2243,7 @@
         <v>43</v>
       </c>
       <c r="M2" t="s">
-        <v>374</v>
+        <v>223</v>
       </c>
       <c r="N2" t="s">
         <v>31</v>
@@ -2627,31 +2266,30 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="30.95703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.1640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.60546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.46484375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.95703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="41.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="40" customWidth="1" collapsed="1"/>
+    <col min="18" max="20" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -2707,66 +2345,66 @@
         <v>75</v>
       </c>
       <c r="R1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="S1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="T1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="U1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="V1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="W1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="X1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" ht="25.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>339</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>195</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G2" t="s">
-        <v>334</v>
+        <v>196</v>
       </c>
       <c r="H2" t="s">
-        <v>335</v>
+        <v>197</v>
       </c>
       <c r="I2" t="s">
-        <v>336</v>
+        <v>198</v>
       </c>
       <c r="J2" t="s">
         <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>337</v>
+        <v>199</v>
       </c>
       <c r="L2" t="s">
-        <v>338</v>
+        <v>200</v>
       </c>
       <c r="M2" t="s">
         <v>31</v>
@@ -2778,34 +2416,34 @@
         <v>33</v>
       </c>
       <c r="P2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="Q2" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="U2" t="s">
         <v>148</v>
       </c>
-      <c r="R2" t="s">
+      <c r="V2" t="s">
+        <v>150</v>
+      </c>
+      <c r="W2" t="s">
+        <v>149</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="S2" t="s">
-        <v>152</v>
-      </c>
-      <c r="T2" t="s">
-        <v>153</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="Y2" t="s">
         <v>160</v>
-      </c>
-      <c r="V2" t="s">
-        <v>162</v>
-      </c>
-      <c r="W2" t="s">
-        <v>161</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2818,32 +2456,32 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:AA2"/>
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.015625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.05859375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.18359375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.04296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.82421875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.95703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.80859375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.44921875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.39453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.86328125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="34.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -2902,28 +2540,28 @@
         <v>75</v>
       </c>
       <c r="S1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="T1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="U1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="V1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="W1" t="s">
         <v>15</v>
       </c>
       <c r="X1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="Y1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="Z1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AA1" t="s">
         <v>69</v>
@@ -2931,31 +2569,31 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>348</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>342</v>
+        <v>204</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>341</v>
+        <v>203</v>
       </c>
       <c r="G2" t="s">
-        <v>343</v>
+        <v>205</v>
       </c>
       <c r="H2" t="s">
-        <v>344</v>
+        <v>206</v>
       </c>
       <c r="I2" t="s">
-        <v>345</v>
+        <v>207</v>
       </c>
       <c r="J2" t="s">
         <v>34</v>
@@ -2964,10 +2602,10 @@
         <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>346</v>
+        <v>208</v>
       </c>
       <c r="M2" t="s">
-        <v>347</v>
+        <v>209</v>
       </c>
       <c r="N2" t="s">
         <v>31</v>
@@ -2979,31 +2617,31 @@
         <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="R2" t="s">
+        <v>139</v>
+      </c>
+      <c r="S2" t="s">
+        <v>152</v>
+      </c>
+      <c r="T2" t="s">
+        <v>153</v>
+      </c>
+      <c r="U2" t="s">
+        <v>154</v>
+      </c>
+      <c r="V2" t="s">
         <v>148</v>
-      </c>
-      <c r="S2" t="s">
-        <v>164</v>
-      </c>
-      <c r="T2" t="s">
-        <v>165</v>
-      </c>
-      <c r="U2" t="s">
-        <v>166</v>
-      </c>
-      <c r="V2" t="s">
-        <v>160</v>
       </c>
       <c r="W2">
         <v>48698</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="AA2" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3016,31 +2654,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF52901-90FE-455B-BEA8-FC50D01098D5}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="41.28515625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="38.42578125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="39.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.42578125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="39.5703125" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -3072,13 +2711,13 @@
         <v>22</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>238</v>
+        <v>166</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>239</v>
+        <v>167</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>240</v>
+        <v>168</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>19</v>
@@ -3099,28 +2738,28 @@
         <v>75</v>
       </c>
       <c r="S1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="T1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="U1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="V1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="W1" t="s">
         <v>15</v>
       </c>
       <c r="X1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="Y1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="Z1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AA1" t="s">
         <v>69</v>
@@ -3128,31 +2767,31 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="G2" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="H2" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="I2" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="J2" t="s">
         <v>34</v>
@@ -3161,10 +2800,10 @@
         <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="M2" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="N2" t="s">
         <v>31</v>
@@ -3176,31 +2815,37 @@
         <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="R2" t="s">
+        <v>139</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="V2" t="s">
         <v>148</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="V2" t="s">
-        <v>160</v>
       </c>
       <c r="W2">
         <v>48698</v>
       </c>
+      <c r="X2" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>156</v>
+      </c>
       <c r="Z2" s="5" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="AA2" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3219,20 +2864,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.01953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.4921875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3284,34 +2929,34 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="G2" t="s">
-        <v>367</v>
+        <v>235</v>
       </c>
       <c r="H2" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="I2" t="s">
-        <v>218</v>
+        <v>241</v>
       </c>
       <c r="J2" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="K2" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="L2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
rectified date picker issues
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="282">
   <si>
     <t>UserName</t>
   </si>
@@ -858,12 +858,34 @@
   </si>
   <si>
     <t>S03.1</t>
+  </si>
+  <si>
+    <t>Automation V2 Project7288747</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>13210 Young Crossroad</t>
+  </si>
+  <si>
+    <t>Carterside</t>
+  </si>
+  <si>
+    <t>74228</t>
+  </si>
+  <si>
+    <t>46899</t>
+  </si>
+  <si>
+    <t>2202278615</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1225,8 +1247,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1301,52 +1323,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="22" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="21" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1328125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.18359375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47">
@@ -1491,10 +1513,10 @@
     </row>
     <row r="2" spans="1:47">
       <c r="A2" s="4" t="s">
-        <v>206</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>275</v>
       </c>
       <c r="C2" t="s">
         <v>209</v>
@@ -1503,22 +1525,22 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>276</v>
       </c>
       <c r="F2" t="s">
-        <v>202</v>
+        <v>277</v>
       </c>
       <c r="G2" t="s">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="H2" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>205</v>
+        <v>280</v>
       </c>
       <c r="K2" t="s">
         <v>179</v>
@@ -1754,37 +1776,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="41.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -2106,18 +2128,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2214,22 +2236,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -2348,25 +2370,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="40" customWidth="1" collapsed="1"/>
-    <col min="18" max="20" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="31.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="18" max="20" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -2538,27 +2560,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -2737,27 +2759,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.42578125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="39.5703125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="39.5703125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -2942,25 +2964,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">

</xml_diff>

<commit_message>
fix for portfolio update
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51400D4-FA99-447A-AA7F-7974063BD4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE7600A-1C64-451A-B607-21521CFE3635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="285">
   <si>
     <t>UserName</t>
   </si>
@@ -635,27 +635,6 @@
     <t>Louisiana</t>
   </si>
   <si>
-    <t>Automation V2 Project3853181</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>7498 Shondra Land</t>
-  </si>
-  <si>
-    <t>New Renaemouth</t>
-  </si>
-  <si>
-    <t>89550-5149</t>
-  </si>
-  <si>
-    <t>22084</t>
-  </si>
-  <si>
-    <t>2202276019</t>
-  </si>
-  <si>
     <t>Elfrieda</t>
   </si>
   <si>
@@ -773,9 +752,6 @@
     <t>46295</t>
   </si>
   <si>
-    <t>WELLP07902</t>
-  </si>
-  <si>
     <t>Akiko</t>
   </si>
   <si>
@@ -879,6 +855,39 @@
   </si>
   <si>
     <t>2202278615</t>
+  </si>
+  <si>
+    <t>ExternalReview</t>
+  </si>
+  <si>
+    <t>Automation portfolio 622990</t>
+  </si>
+  <si>
+    <t>19432</t>
+  </si>
+  <si>
+    <t>05936 Runolfsdottir Crossing</t>
+  </si>
+  <si>
+    <t>Mosesmouth</t>
+  </si>
+  <si>
+    <t>75723-3548</t>
+  </si>
+  <si>
+    <t>WELLP08258</t>
+  </si>
+  <si>
+    <t>Rickey</t>
+  </si>
+  <si>
+    <t>cicely.orn@gmail.com</t>
+  </si>
+  <si>
+    <t>3325632315</t>
+  </si>
+  <si>
+    <t>Latoya</t>
   </si>
 </sst>
 </file>
@@ -1323,16 +1332,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1328125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.18359375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
@@ -1513,46 +1521,46 @@
     </row>
     <row r="2" spans="1:47">
       <c r="A2" s="4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="F2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="G2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="H2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="K2" t="s">
         <v>179</v>
       </c>
       <c r="L2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="M2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="N2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="O2" t="s">
         <v>29</v>
@@ -1561,19 +1569,19 @@
         <v>198</v>
       </c>
       <c r="Q2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="R2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="S2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="T2" t="s">
+        <v>200</v>
+      </c>
+      <c r="U2" t="s">
         <v>207</v>
-      </c>
-      <c r="U2" t="s">
-        <v>214</v>
       </c>
       <c r="V2" t="s">
         <v>31</v>
@@ -1768,37 +1776,37 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA429754-6532-434F-8D5F-1B15F28EE35F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.62890625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.50390625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="27.1171875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.80078125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.27734375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.25" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.29296875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="25.97265625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
     <col min="20" max="20" customWidth="true" width="28.140625" collapsed="true"/>
     <col min="21" max="21" customWidth="true" width="34.7109375" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="41.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="34.7109375" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="26" max="26" customWidth="true" width="37.5703125" collapsed="true"/>
@@ -1807,9 +1815,10 @@
     <col min="30" max="30" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
     <col min="31" max="31" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
     <col min="33" max="33" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="34.203125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1877,51 +1886,54 @@
         <v>126</v>
       </c>
       <c r="W1" t="s">
+        <v>274</v>
+      </c>
+      <c r="X1" t="s">
         <v>78</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>127</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>128</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>129</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>130</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>140</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>141</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>142</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>90</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="30">
+    <row r="2" spans="1:34" ht="105">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>275</v>
       </c>
       <c r="C2" t="s">
         <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>59</v>
@@ -1930,34 +1942,34 @@
         <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="J2" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
       <c r="K2" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="L2" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="M2" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
       <c r="N2" t="s">
-        <v>248</v>
+        <v>282</v>
       </c>
       <c r="O2" t="s">
-        <v>249</v>
+        <v>283</v>
       </c>
       <c r="P2" t="s">
-        <v>250</v>
+        <v>284</v>
       </c>
       <c r="Q2" t="s">
         <v>31</v>
@@ -1978,45 +1990,48 @@
         <v>159</v>
       </c>
       <c r="W2" t="s">
+        <v>159</v>
+      </c>
+      <c r="X2" t="s">
         <v>134</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>133</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>135</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>132</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>143</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>144</v>
       </c>
-      <c r="AD2" t="s">
-        <v>239</v>
-      </c>
       <c r="AE2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF2" t="s">
         <v>151</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AG2" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="30">
+    <row r="3" spans="1:34" ht="105">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
         <v>171</v>
@@ -2031,7 +2046,7 @@
         <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -2040,25 +2055,25 @@
         <v>197</v>
       </c>
       <c r="J3" t="s">
+        <v>224</v>
+      </c>
+      <c r="K3" t="s">
+        <v>225</v>
+      </c>
+      <c r="L3" t="s">
+        <v>226</v>
+      </c>
+      <c r="M3" t="s">
+        <v>228</v>
+      </c>
+      <c r="N3" t="s">
+        <v>229</v>
+      </c>
+      <c r="O3" t="s">
+        <v>230</v>
+      </c>
+      <c r="P3" t="s">
         <v>231</v>
-      </c>
-      <c r="K3" t="s">
-        <v>232</v>
-      </c>
-      <c r="L3" t="s">
-        <v>233</v>
-      </c>
-      <c r="M3" t="s">
-        <v>235</v>
-      </c>
-      <c r="N3" t="s">
-        <v>236</v>
-      </c>
-      <c r="O3" t="s">
-        <v>237</v>
-      </c>
-      <c r="P3" t="s">
-        <v>238</v>
       </c>
       <c r="Q3" t="s">
         <v>31</v>
@@ -2079,36 +2094,39 @@
         <v>159</v>
       </c>
       <c r="W3" t="s">
+        <v>159</v>
+      </c>
+      <c r="X3" t="s">
         <v>134</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>133</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>135</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>132</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>143</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>144</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>153</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>151</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2470,10 +2488,10 @@
     </row>
     <row r="2" spans="1:25" ht="25.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
         <v>152</v>
@@ -2488,22 +2506,22 @@
         <v>199</v>
       </c>
       <c r="G2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H2" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I2" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="J2" t="s">
         <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="M2" t="s">
         <v>31</v>
@@ -2668,10 +2686,10 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2686,13 +2704,13 @@
         <v>162</v>
       </c>
       <c r="G2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="I2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="J2" t="s">
         <v>34</v>
@@ -2701,10 +2719,10 @@
         <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="M2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="N2" t="s">
         <v>31</v>
@@ -2958,7 +2976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBEA2DE-44FE-4DF1-AA87-197E84162088}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
@@ -3029,19 +3047,19 @@
         <v>71</v>
       </c>
       <c r="O1" t="s">
+        <v>243</v>
+      </c>
+      <c r="P1" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>245</v>
+      </c>
+      <c r="R1" t="s">
+        <v>248</v>
+      </c>
+      <c r="S1" t="s">
         <v>251</v>
-      </c>
-      <c r="P1" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>253</v>
-      </c>
-      <c r="R1" t="s">
-        <v>256</v>
-      </c>
-      <c r="S1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -3049,13 +3067,13 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -3064,19 +3082,19 @@
         <v>199</v>
       </c>
       <c r="G2" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="K2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="L2" t="s">
         <v>31</v>
@@ -3088,53 +3106,53 @@
         <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="P2" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="R2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="S2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="O3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="P3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="Q3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="R3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="S3" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="O4" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="P4" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="Q4" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="R4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="S4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix portfolio filter list
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WellFrontendTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F76D49-687C-45F7-B905-52795B9D36E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193944F5-E994-4A67-8589-357DF642D4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="344">
   <si>
     <t>UserName</t>
   </si>
@@ -863,285 +863,9 @@
     <t>India</t>
   </si>
   <si>
-    <t>Automation V2 Project5480455</t>
-  </si>
-  <si>
-    <t>Lakshadweep</t>
-  </si>
-  <si>
-    <t>06598 Samual Ville</t>
-  </si>
-  <si>
-    <t>Port Salvadorburgh</t>
-  </si>
-  <si>
-    <t>42561</t>
-  </si>
-  <si>
-    <t>70146</t>
-  </si>
-  <si>
-    <t>2202279962</t>
-  </si>
-  <si>
-    <t>Arnulfo</t>
-  </si>
-  <si>
-    <t>wilford.feest@gmail.com</t>
-  </si>
-  <si>
-    <t>2914730876</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>41606 Carie Falls</t>
-  </si>
-  <si>
-    <t>Hermannfort</t>
-  </si>
-  <si>
-    <t>40721</t>
-  </si>
-  <si>
-    <t>Leola</t>
-  </si>
-  <si>
-    <t>Automation V2 Project5006648</t>
-  </si>
-  <si>
-    <t>Andhra Pradesh</t>
-  </si>
-  <si>
-    <t>077 Ronald Lakes</t>
-  </si>
-  <si>
-    <t>South Genevieve</t>
-  </si>
-  <si>
-    <t>46927</t>
-  </si>
-  <si>
-    <t>76437</t>
-  </si>
-  <si>
-    <t>2202279963</t>
-  </si>
-  <si>
-    <t>Gena</t>
-  </si>
-  <si>
-    <t>mallie.stark@yahoo.com</t>
-  </si>
-  <si>
-    <t>6547528476</t>
-  </si>
-  <si>
-    <t>Museums, Libraries</t>
-  </si>
-  <si>
-    <t>Assam</t>
-  </si>
-  <si>
-    <t>302 Crist Creek</t>
-  </si>
-  <si>
-    <t>East Drema</t>
-  </si>
-  <si>
-    <t>32398-2091</t>
-  </si>
-  <si>
-    <t>Arron</t>
-  </si>
-  <si>
-    <t>Automation V2 Project3143145</t>
-  </si>
-  <si>
-    <t>Jammu and Kashmir</t>
-  </si>
-  <si>
-    <t>471 Keenan Cove</t>
-  </si>
-  <si>
-    <t>Kirlinmouth</t>
-  </si>
-  <si>
-    <t>23503</t>
-  </si>
-  <si>
-    <t>56319</t>
-  </si>
-  <si>
-    <t>2202279972</t>
-  </si>
-  <si>
     <t>1-800 Flowers.com Inc.</t>
   </si>
   <si>
-    <t>Shad</t>
-  </si>
-  <si>
-    <t>kym.altenwerth@yahoo.com</t>
-  </si>
-  <si>
-    <t>3700882608</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>531 Summer Square</t>
-  </si>
-  <si>
-    <t>Nicolasland</t>
-  </si>
-  <si>
-    <t>02385</t>
-  </si>
-  <si>
-    <t>Bridget</t>
-  </si>
-  <si>
-    <t>Automation V2 Project558979</t>
-  </si>
-  <si>
-    <t>Chandigarh</t>
-  </si>
-  <si>
-    <t>3751 Mertz Ranch</t>
-  </si>
-  <si>
-    <t>Strackebury</t>
-  </si>
-  <si>
-    <t>14665</t>
-  </si>
-  <si>
-    <t>13728</t>
-  </si>
-  <si>
-    <t>2202279973</t>
-  </si>
-  <si>
-    <t>Heriberto</t>
-  </si>
-  <si>
-    <t>abel.ernser@gmail.com</t>
-  </si>
-  <si>
-    <t>4898950521</t>
-  </si>
-  <si>
-    <t>Uttaranchal</t>
-  </si>
-  <si>
-    <t>80226 Steuber Overpass</t>
-  </si>
-  <si>
-    <t>Lucyville</t>
-  </si>
-  <si>
-    <t>19170</t>
-  </si>
-  <si>
-    <t>Rose</t>
-  </si>
-  <si>
-    <t>Automation V2 Project5832015</t>
-  </si>
-  <si>
-    <t>Bihar</t>
-  </si>
-  <si>
-    <t>703 Lawanda Path</t>
-  </si>
-  <si>
-    <t>Rempelfurt</t>
-  </si>
-  <si>
-    <t>65378-4339</t>
-  </si>
-  <si>
-    <t>23462</t>
-  </si>
-  <si>
-    <t>2202279974</t>
-  </si>
-  <si>
-    <t>Blossom</t>
-  </si>
-  <si>
-    <t>tandra.okuneva@yahoo.com</t>
-  </si>
-  <si>
-    <t>0384688030</t>
-  </si>
-  <si>
-    <t>Ground Travel</t>
-  </si>
-  <si>
-    <t>Jharkhand</t>
-  </si>
-  <si>
-    <t>04166 Inga Park</t>
-  </si>
-  <si>
-    <t>Port Phillip</t>
-  </si>
-  <si>
-    <t>30899</t>
-  </si>
-  <si>
-    <t>Odis</t>
-  </si>
-  <si>
-    <t>Automation V2 Project3070114</t>
-  </si>
-  <si>
-    <t>Punjab</t>
-  </si>
-  <si>
-    <t>843 Robin Loop</t>
-  </si>
-  <si>
-    <t>West Baileybury</t>
-  </si>
-  <si>
-    <t>10025-6653</t>
-  </si>
-  <si>
-    <t>36054</t>
-  </si>
-  <si>
-    <t>2202279975</t>
-  </si>
-  <si>
-    <t>Flossie</t>
-  </si>
-  <si>
-    <t>ilse.daniel@yahoo.com</t>
-  </si>
-  <si>
-    <t>4058685880</t>
-  </si>
-  <si>
-    <t>Media, PR &amp; Communications</t>
-  </si>
-  <si>
-    <t>532 Thompson Points</t>
-  </si>
-  <si>
-    <t>Kassieburgh</t>
-  </si>
-  <si>
-    <t>99294</t>
-  </si>
-  <si>
-    <t>Ramiro</t>
-  </si>
-  <si>
     <t>Automation V2 Project1193912</t>
   </si>
   <si>
@@ -1188,6 +912,159 @@
   </si>
   <si>
     <t>Candace</t>
+  </si>
+  <si>
+    <t>Automation portfolio 73759</t>
+  </si>
+  <si>
+    <t>Hospitals</t>
+  </si>
+  <si>
+    <t>12082</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>003 Huel Manor</t>
+  </si>
+  <si>
+    <t>Lake Keiko</t>
+  </si>
+  <si>
+    <t>27001-0906</t>
+  </si>
+  <si>
+    <t>WELLP08317</t>
+  </si>
+  <si>
+    <t>Cristopher</t>
+  </si>
+  <si>
+    <t>sherell.pollich@yahoo.com</t>
+  </si>
+  <si>
+    <t>1683614727</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Automation portfolio 1046908</t>
+  </si>
+  <si>
+    <t>REIT</t>
+  </si>
+  <si>
+    <t>30752</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>9134 Schiller Cliffs</t>
+  </si>
+  <si>
+    <t>Hobertmouth</t>
+  </si>
+  <si>
+    <t>06293</t>
+  </si>
+  <si>
+    <t>WELLP08318</t>
+  </si>
+  <si>
+    <t>Cody</t>
+  </si>
+  <si>
+    <t>jerilyn.nikolaus@gmail.com</t>
+  </si>
+  <si>
+    <t>6870785311</t>
+  </si>
+  <si>
+    <t>Hollis</t>
+  </si>
+  <si>
+    <t>Automation portfolio 5614492</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>63785 Botsford Flat</t>
+  </si>
+  <si>
+    <t>Port Levimouth</t>
+  </si>
+  <si>
+    <t>46539</t>
+  </si>
+  <si>
+    <t>WELLP08319</t>
+  </si>
+  <si>
+    <t>Theda</t>
+  </si>
+  <si>
+    <t>renato.zieme@gmail.com</t>
+  </si>
+  <si>
+    <t>1646262927</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>Automation portfolio 922742</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>37040</t>
+  </si>
+  <si>
+    <t>0134 Melvin Plain</t>
+  </si>
+  <si>
+    <t>Lake Clarisa</t>
+  </si>
+  <si>
+    <t>21615</t>
+  </si>
+  <si>
+    <t>WELLP08321</t>
+  </si>
+  <si>
+    <t>Pamula</t>
+  </si>
+  <si>
+    <t>ernest.jacobs@gmail.com</t>
+  </si>
+  <si>
+    <t>2102883632</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Automation portfolio 2694740</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>17402</t>
+  </si>
+  <si>
+    <t>Missouri</t>
   </si>
 </sst>
 </file>
@@ -1626,33 +1503,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DDA08-C4FB-4E43-ADE7-EDDAA41E68CF}">
   <dimension ref="A1:AU4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4:X4"/>
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.24609375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.12890625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.14453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.6484375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="62.921875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.61328125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.6953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="27.5546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="27.66796875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.23046875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.71875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.41015625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.82421875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.12109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="62.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
@@ -2067,67 +1944,67 @@
     </row>
     <row r="4" spans="1:47">
       <c r="A4" t="s">
-        <v>375</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>369</v>
+        <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>378</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
         <v>275</v>
       </c>
       <c r="E4" t="s">
-        <v>370</v>
+        <v>278</v>
       </c>
       <c r="F4" t="s">
-        <v>371</v>
+        <v>279</v>
       </c>
       <c r="G4" t="s">
-        <v>372</v>
+        <v>280</v>
       </c>
       <c r="H4" t="s">
-        <v>373</v>
+        <v>281</v>
       </c>
       <c r="I4" t="s">
         <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>374</v>
+        <v>282</v>
       </c>
       <c r="K4" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="L4" t="s">
-        <v>376</v>
+        <v>284</v>
       </c>
       <c r="M4" t="s">
-        <v>377</v>
+        <v>285</v>
       </c>
       <c r="N4" t="s">
-        <v>379</v>
+        <v>287</v>
       </c>
       <c r="O4" t="s">
         <v>275</v>
       </c>
       <c r="P4" t="s">
-        <v>380</v>
+        <v>288</v>
       </c>
       <c r="Q4" t="s">
-        <v>381</v>
+        <v>289</v>
       </c>
       <c r="R4" t="s">
-        <v>382</v>
+        <v>290</v>
       </c>
       <c r="S4" t="s">
-        <v>383</v>
+        <v>291</v>
       </c>
       <c r="T4" t="s">
-        <v>376</v>
+        <v>284</v>
       </c>
       <c r="U4" t="s">
-        <v>384</v>
+        <v>292</v>
       </c>
       <c r="V4" t="s">
         <v>31</v>
@@ -2148,30 +2025,30 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA429754-6532-434F-8D5F-1B15F28EE35F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.62890625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.35546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.50390625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="27.1171875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.80078125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.27734375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="26.890625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.29296875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.74609375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.41015625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="25.015625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.7890625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.56640625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
@@ -2500,6 +2377,65 @@
       </c>
       <c r="AH3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
+      <c r="A4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>342</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>343</v>
+      </c>
+      <c r="J4" t="s">
+        <v>332</v>
+      </c>
+      <c r="K4" t="s">
+        <v>333</v>
+      </c>
+      <c r="L4" t="s">
+        <v>334</v>
+      </c>
+      <c r="M4" t="s">
+        <v>336</v>
+      </c>
+      <c r="N4" t="s">
+        <v>337</v>
+      </c>
+      <c r="O4" t="s">
+        <v>338</v>
+      </c>
+      <c r="P4" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>